<commit_message>
moved U2 and S33-S35
</commit_message>
<xml_diff>
--- a/KiCadHacks.xlsx
+++ b/KiCadHacks.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JRo\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\kiibohd-pcb\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3000" windowWidth="23720" windowHeight="5180" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="4800" windowWidth="23720" windowHeight="5180"/>
   </bookViews>
   <sheets>
     <sheet name="MoveSW" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="32">
   <si>
     <t>X</t>
   </si>
@@ -73,30 +73,12 @@
     <t>Θ</t>
   </si>
   <si>
-    <t xml:space="preserve">    (at 165.334 117.82 155)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  (gr_line (start 100.888898 135.337045) (end 86.941176 134.116777) (layer Dwgs.User) (width 0.1))</t>
-  </si>
-  <si>
     <t>start</t>
   </si>
   <si>
     <t>end</t>
   </si>
   <si>
-    <t xml:space="preserve">  (gr_line (start 85.720917 148.0644) (end 99.668639 149.284667) (layer Dwgs.User) (width 0.1))</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    (at 162.514 116.505 155)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    (at 167.483 113.215 335)</t>
-  </si>
-  <si>
-    <t>U1</t>
-  </si>
-  <si>
     <t xml:space="preserve">at </t>
   </si>
   <si>
@@ -109,17 +91,46 @@
     <t>R2</t>
   </si>
   <si>
-    <t xml:space="preserve">    (at 136.525 125.984 180)</t>
+    <t xml:space="preserve">  (gr_line (start 57.4675 122.9155) (end 57.4675 119.8145) (layer Dwgs.User) (width 0.1))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">start </t>
+  </si>
+  <si>
+    <t xml:space="preserve">end </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  (gr_line (start 80.481628 118.595728) (end 79.976212 124.372662) (layer Dwgs.User) (width 0.1))</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    (at 116.332 126.111 180)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  (gr_line (start 118.033061 131.010419) (end 117.026076 136.721319) (layer Dwgs.User) (width 0.1))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  (gr_line (start 130.814369 139.152568) (end 131.821355 133.441667) (layer Dwgs.User) (width 0.1))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    (at 135.994 135.666 65)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    (at 137.31 132.847 65)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    (at 140.597 137.813 245)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.000000"/>
-    <numFmt numFmtId="166" formatCode="0.00000"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -224,7 +235,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -234,6 +244,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -550,8 +561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:D2"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -583,7 +594,7 @@
         <v>14</v>
       </c>
       <c r="F2" s="6">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="Q2" s="2" t="s">
         <v>0</v>
@@ -597,7 +608,7 @@
       <c r="T2" s="2"/>
       <c r="U2" s="2"/>
       <c r="V2" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
@@ -605,22 +616,22 @@
     <row r="3" spans="1:26" x14ac:dyDescent="0.35">
       <c r="B3">
         <f>IFERROR(VALUE(MID($G3,L3,M3-L3)),VALUE(RIGHT($G3,LEN($G3)-L3)))</f>
-        <v>165.334</v>
+        <v>135.994</v>
       </c>
       <c r="C3">
         <f t="shared" ref="C3" si="0">IFERROR(VALUE(MID($G3,M3,N3-M3)),VALUE(RIGHT($G3,LEN($G3)-M3)))</f>
-        <v>117.82</v>
+        <v>135.666</v>
       </c>
       <c r="D3">
         <f>IFERROR(VALUE(MID($G3,N3,O3-N3)),VALUE(MID($G3,N3,LEN($G3)-N3)))</f>
-        <v>155</v>
+        <v>65</v>
       </c>
       <c r="F3" t="str">
         <f>"S"&amp;F2</f>
-        <v>S22</v>
+        <v>S33</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="H3" s="1">
         <f>FIND(" ",$G3)</f>
@@ -648,7 +659,7 @@
       </c>
       <c r="N3" s="1">
         <f t="shared" ref="N3" si="5">FIND(" ",$G3,M3+1)</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="O3" s="1" t="e">
         <f t="shared" ref="O3" si="6">FIND(" ",$G3,N3+1)</f>
@@ -656,18 +667,18 @@
       </c>
       <c r="Q3">
         <f>AVERAGE(Q6:Q9)</f>
-        <v>93.304907499999999</v>
+        <v>124.42371525000001</v>
       </c>
       <c r="R3">
         <f>AVERAGE(R6:R9)</f>
-        <v>141.70072225000001</v>
+        <v>135.08149324999999</v>
       </c>
       <c r="S3">
-        <f>DEGREES(ASIN(R4/S4))</f>
-        <v>5.0000018059286759</v>
+        <f>90+ROUND(DEGREES(ASIN(R4/S4)),2)</f>
+        <v>10</v>
       </c>
       <c r="V3" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="W3" s="1"/>
       <c r="X3" s="1"/>
@@ -677,35 +688,35 @@
     <row r="4" spans="1:26" x14ac:dyDescent="0.35">
       <c r="B4">
         <f>Q3</f>
-        <v>93.304907499999999</v>
+        <v>124.42371525000001</v>
       </c>
       <c r="C4">
         <f>R3</f>
-        <v>141.70072225000001</v>
+        <v>135.08149324999999</v>
       </c>
       <c r="D4" s="7">
         <f>180-S3</f>
-        <v>174.99999819407134</v>
+        <v>170</v>
       </c>
       <c r="F4" t="str">
         <f>F3&amp;"'"</f>
-        <v>S22'</v>
+        <v>S33'</v>
       </c>
       <c r="G4" t="str">
         <f>LEFT(G3,L3)&amp;TEXT(B4,"#0.0####")&amp;" "&amp;TEXT(C4,"#0.0####")&amp;" "&amp;TEXT(D4,"#0")&amp;")"</f>
-        <v xml:space="preserve">    (at 93.30491 141.70072 175)</v>
+        <v xml:space="preserve">    (at 124.42372 135.08149 170)</v>
       </c>
       <c r="Q4">
         <f>ABS(Q6-Q7)</f>
-        <v>13.947721999999999</v>
-      </c>
-      <c r="R4">
+        <v>1.0069850000000002</v>
+      </c>
+      <c r="R4" s="9">
         <f>(R6-R7)</f>
-        <v>1.2202679999999759</v>
+        <v>-5.710899999999981</v>
       </c>
       <c r="S4" s="5">
         <f>SQRT(Q4^2+R4^2)</f>
-        <v>14.0010000707488</v>
+        <v>5.7989997068653825</v>
       </c>
       <c r="V4" s="1"/>
       <c r="W4" s="1"/>
@@ -724,7 +735,7 @@
       </c>
       <c r="D5">
         <f>D4-D3</f>
-        <v>19.999998194071338</v>
+        <v>105</v>
       </c>
       <c r="H5" s="1" t="e">
         <f>FIND(" ",$G5)</f>
@@ -742,26 +753,26 @@
     <row r="6" spans="1:26" x14ac:dyDescent="0.35">
       <c r="B6" s="5">
         <f>B4-B3</f>
-        <v>-72.029092500000004</v>
+        <v>-11.570284749999985</v>
       </c>
       <c r="C6" s="5">
         <f>C4-C3</f>
-        <v>23.880722250000019</v>
+        <v>-0.58450675000000274</v>
       </c>
       <c r="D6" s="5">
         <f>ROUND(S3,2)</f>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="Q6" s="9">
         <f>VALUE(MID($U$6,V6+1,W6-V6))</f>
-        <v>100.888898</v>
+        <v>118.033061</v>
       </c>
       <c r="R6" s="9">
         <f>VALUE(MID($U$6,W6+1,X6-W6-1))</f>
-        <v>135.33704499999999</v>
+        <v>131.01041900000001</v>
       </c>
       <c r="U6" s="1" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="V6" s="1">
         <f>FIND(V2,$U$6)+LEN(V2)</f>
@@ -779,23 +790,26 @@
     <row r="7" spans="1:26" x14ac:dyDescent="0.35">
       <c r="B7" s="5">
         <f>B10-B3</f>
-        <v>-2.8199999999999932</v>
+        <v>1.3160000000000025</v>
       </c>
       <c r="C7" s="5">
         <f>C10-C3</f>
-        <v>-1.3149999999999977</v>
+        <v>-2.8189999999999884</v>
       </c>
       <c r="D7" s="5">
         <f>SQRT(B7^2+C7^2)</f>
-        <v>3.1115309736526737</v>
+        <v>3.1110475727638658</v>
+      </c>
+      <c r="E7" s="1">
+        <v>-1</v>
       </c>
       <c r="Q7" s="9">
         <f>VALUE(MID($U$6,V7+1,W7-V7))</f>
-        <v>86.941175999999999</v>
+        <v>117.026076</v>
       </c>
       <c r="R7" s="9">
         <f>VALUE(MID($U$6,W7+1,X7-W7-1))</f>
-        <v>134.11677700000001</v>
+        <v>136.72131899999999</v>
       </c>
       <c r="V7" s="1">
         <f>FIND(V3,$U$6)+LEN(V3)</f>
@@ -803,35 +817,35 @@
       </c>
       <c r="W7" s="1">
         <f>FIND(" ",$U$6,V7+1)</f>
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="X7" s="1">
         <f>FIND(")",$U$6,W7+1)</f>
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.35">
       <c r="B8" s="5">
-        <f>-B7-$D7*COS(RADIANS($D6))</f>
-        <v>-0.27969065890104705</v>
+        <f>E7*(B7+$D7*COS(RADIANS($D6)))</f>
+        <v>-4.3797837696476689</v>
       </c>
       <c r="C8" s="5">
         <f>E8*(C7+$D7*SIN(RADIANS($D6)))</f>
-        <v>1.0438122069089548</v>
+        <v>2.2787722583544161</v>
       </c>
       <c r="E8" s="1">
         <v>-1</v>
       </c>
       <c r="Q8" s="9">
         <f>VALUE(MID($U$8,V8+1,W8-V8))</f>
-        <v>85.720917</v>
+        <v>130.814369</v>
       </c>
       <c r="R8" s="9">
         <f>VALUE(MID($U$8,W8+1,X8-W8-1))</f>
-        <v>148.06440000000001</v>
+        <v>139.152568</v>
       </c>
       <c r="U8" s="1" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="V8" s="1">
         <f>FIND(V2,$U$8)+LEN(V2)</f>
@@ -839,11 +853,11 @@
       </c>
       <c r="W8" s="1">
         <f>FIND(" ",$U$8,V8+1)</f>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="X8" s="1">
         <f>FIND(")",$U$8,W8+1)</f>
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.35">
@@ -851,44 +865,44 @@
       <c r="C9" s="5"/>
       <c r="Q9" s="9">
         <f>VALUE(MID($U$8,V9+1,W9-V9))</f>
-        <v>99.668638999999999</v>
+        <v>131.82135500000001</v>
       </c>
       <c r="R9" s="9">
         <f>VALUE(MID($U$8,W9+1,X9-W9-1))</f>
-        <v>149.28466700000001</v>
+        <v>133.441667</v>
       </c>
       <c r="V9" s="1">
         <f>FIND(V3,$U$8)+LEN(V3)</f>
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="W9" s="1">
         <f>FIND(" ",$U$8,V9+1)</f>
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="X9" s="1">
         <f>FIND(")",$U$8,W9+1)</f>
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.35">
       <c r="B10">
         <f>IFERROR(VALUE(MID($G10,L10,M10-L10)),VALUE(RIGHT($G10,LEN($G10)-L10)))</f>
-        <v>162.51400000000001</v>
+        <v>137.31</v>
       </c>
       <c r="C10">
         <f t="shared" ref="C10" si="7">IFERROR(VALUE(MID($G10,M10,N10-M10)),VALUE(RIGHT($G10,LEN($G10)-M10)))</f>
-        <v>116.505</v>
+        <v>132.84700000000001</v>
       </c>
       <c r="D10">
         <f>IFERROR(VALUE(MID($G10,N10,O10-N10)),VALUE(MID($G10,N10,LEN($G10)-N10)))</f>
-        <v>155</v>
+        <v>65</v>
       </c>
       <c r="F10" t="str">
         <f>"D"&amp;F2</f>
-        <v>D22</v>
+        <v>D33</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H10" s="1">
         <f>FIND(" ",$G10)</f>
@@ -912,11 +926,11 @@
       </c>
       <c r="M10" s="1">
         <f t="shared" si="8"/>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N10" s="1">
         <f t="shared" si="8"/>
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O10" s="1" t="e">
         <f t="shared" si="8"/>
@@ -926,45 +940,45 @@
     <row r="11" spans="1:26" x14ac:dyDescent="0.35">
       <c r="B11">
         <f>B10+B$6+B8</f>
-        <v>90.205216841098959</v>
+        <v>121.35993148035234</v>
       </c>
       <c r="C11">
         <f>C10+C$6+C8</f>
-        <v>141.42953445690898</v>
+        <v>134.54126550835443</v>
       </c>
       <c r="D11">
         <f>IF(D10+D$5&lt;0,360+D10+D$5,D10+D$5)</f>
-        <v>174.99999819407134</v>
+        <v>170</v>
       </c>
       <c r="F11" t="str">
         <f>F10&amp;"'"</f>
-        <v>D22'</v>
+        <v>D33'</v>
       </c>
       <c r="G11" t="str">
         <f>LEFT(G10,L10)&amp;TEXT(B11,"#0.0####")&amp;" "&amp;TEXT(C11,"#0.0####")&amp;" "&amp;TEXT(D11,"#0")&amp;")"</f>
-        <v xml:space="preserve">    (at 90.20522 141.42953 175)</v>
+        <v xml:space="preserve">    (at 121.35993 134.54127 170)</v>
       </c>
       <c r="V11" s="8"/>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.35">
       <c r="B13">
         <f>IFERROR(VALUE(MID($G13,L13,M13-L13)),VALUE(RIGHT($G13,LEN($G13)-L13)))</f>
-        <v>167.483</v>
+        <v>140.59700000000001</v>
       </c>
       <c r="C13">
         <f t="shared" ref="C13" si="9">IFERROR(VALUE(MID($G13,M13,N13-M13)),VALUE(RIGHT($G13,LEN($G13)-M13)))</f>
-        <v>113.215</v>
+        <v>137.81299999999999</v>
       </c>
       <c r="D13">
         <f>IFERROR(VALUE(MID($G13,N13,O13-N13)),VALUE(MID($G13,N13,LEN($G13)-N13)))</f>
-        <v>335</v>
+        <v>245</v>
       </c>
       <c r="F13" t="str">
         <f>"D"&amp;TEXT(F2+F16,"0")</f>
-        <v>D60</v>
+        <v>D71</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="H13" s="1">
         <f>FIND(" ",$G13)</f>
@@ -1001,24 +1015,24 @@
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.35">
       <c r="B14">
-        <f>B13+B$6+B17*A17</f>
-        <v>93.716445322367832</v>
+        <f>B4+B17</f>
+        <v>125.30584799254802</v>
       </c>
       <c r="C14">
-        <f>C13+C$6+C17</f>
-        <v>136.78936081835622</v>
+        <f>C4+C17+C16</f>
+        <v>129.92431663530203</v>
       </c>
       <c r="D14">
         <f>IF(D13+D$5&lt;0,360+D13+D$5,D13+D$5)</f>
-        <v>354.99999819407134</v>
+        <v>350</v>
       </c>
       <c r="F14" t="str">
         <f>F13&amp;"'"</f>
-        <v>D60'</v>
+        <v>D71'</v>
       </c>
       <c r="G14" t="str">
         <f>LEFT(G13,L13)&amp;TEXT(B14,"#0.0####")&amp;" "&amp;TEXT(C14,"#0.0####")&amp;" "&amp;TEXT(D14,"#0")&amp;")"</f>
-        <v xml:space="preserve">    (at 93.71645 136.78936 355)</v>
+        <v xml:space="preserve">    (at 125.30585 129.92432 350)</v>
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.35">
@@ -1043,12 +1057,12 @@
         <v>-1</v>
       </c>
       <c r="B17" s="5">
-        <f>B16+$D16*SIN(RADIANS($D5))</f>
-        <v>1.7374621776321681</v>
+        <f>B16+$D16*SIN(RADIANS($D6))</f>
+        <v>0.88213274254800578</v>
       </c>
       <c r="C17" s="5">
-        <f>C16+$D16*COS(RADIANS($D5))</f>
-        <v>-0.30636143164381568</v>
+        <f>C16+$D16*COS(RADIANS($D6))</f>
+        <v>-7.717661469798287E-2</v>
       </c>
     </row>
   </sheetData>
@@ -1097,12 +1111,12 @@
       </c>
       <c r="B3" s="5">
         <f>MoveSW!B6</f>
-        <v>-72.029092500000004</v>
+        <v>-11.570284749999985</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5">
         <f>MoveSW!B6</f>
-        <v>-72.029092500000004</v>
+        <v>-11.570284749999985</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="3" t="s">
@@ -1112,7 +1126,7 @@
     <row r="4" spans="1:22" x14ac:dyDescent="0.35">
       <c r="B4">
         <f>VALUE(MID($G4,K4,L4-K4))+B$3</f>
-        <v>-40.203392500000007</v>
+        <v>20.255415250000016</v>
       </c>
       <c r="C4">
         <f>VALUE(MID($G4,L4,M4-L4-1))+C$3</f>
@@ -1120,7 +1134,7 @@
       </c>
       <c r="D4">
         <f>VALUE(MID($G4,N4,O4-N4))+D$3</f>
-        <v>-39.736592500000008</v>
+        <v>20.722215250000012</v>
       </c>
       <c r="E4">
         <f>VALUE(MID($G4,O4,P4-O4-1))+E$3</f>
@@ -1193,7 +1207,7 @@
     <row r="5" spans="1:22" x14ac:dyDescent="0.35">
       <c r="B5">
         <f t="shared" ref="B5:B8" si="1">VALUE(MID($G5,K5,L5-K5))+B$3</f>
-        <v>-40.203392500000007</v>
+        <v>20.255415250000016</v>
       </c>
       <c r="C5">
         <f t="shared" ref="C5:C8" si="2">VALUE(MID($G5,L5,M5-L5-1))+C$3</f>
@@ -1201,7 +1215,7 @@
       </c>
       <c r="D5">
         <f t="shared" ref="D5:D8" si="3">VALUE(MID($G5,N5,O5-N5))+D$3</f>
-        <v>-40.617792500000007</v>
+        <v>19.841015250000016</v>
       </c>
       <c r="E5">
         <f t="shared" ref="E5:E8" si="4">VALUE(MID($G5,O5,P5-O5-1))+E$3</f>
@@ -1430,7 +1444,7 @@
     <row r="8" spans="1:22" x14ac:dyDescent="0.35">
       <c r="B8">
         <f t="shared" si="1"/>
-        <v>-41.975592500000005</v>
+        <v>18.483215250000015</v>
       </c>
       <c r="C8">
         <f t="shared" si="2"/>
@@ -1438,7 +1452,7 @@
       </c>
       <c r="D8">
         <f t="shared" si="3"/>
-        <v>-41.97959250000001</v>
+        <v>18.479215250000014</v>
       </c>
       <c r="E8">
         <f t="shared" si="4"/>
@@ -1511,7 +1525,7 @@
     <row r="9" spans="1:22" x14ac:dyDescent="0.35">
       <c r="B9">
         <f t="shared" ref="B9:B13" si="7">VALUE(MID($G9,K9,L9-K9))+B$3</f>
-        <v>-40.3692925</v>
+        <v>20.089515250000016</v>
       </c>
       <c r="C9">
         <f t="shared" ref="C9:C13" si="8">VALUE(MID($G9,L9,M9-L9-1))+C$3</f>
@@ -1519,7 +1533,7 @@
       </c>
       <c r="D9">
         <f t="shared" ref="D9:D13" si="9">VALUE(MID($G9,N9,O9-N9))+D$3</f>
-        <v>-41.975592500000005</v>
+        <v>18.483215250000015</v>
       </c>
       <c r="E9">
         <f t="shared" ref="E9:E13" si="10">VALUE(MID($G9,O9,P9-O9-1))+E$3</f>
@@ -1592,7 +1606,7 @@
     <row r="10" spans="1:22" x14ac:dyDescent="0.35">
       <c r="B10">
         <f t="shared" si="7"/>
-        <v>-40.188692500000002</v>
+        <v>20.270115250000014</v>
       </c>
       <c r="C10">
         <f t="shared" si="8"/>
@@ -1600,7 +1614,7 @@
       </c>
       <c r="D10">
         <f t="shared" si="9"/>
-        <v>-40.127892500000002</v>
+        <v>20.330915250000015</v>
       </c>
       <c r="E10">
         <f t="shared" si="10"/>
@@ -1673,7 +1687,7 @@
     <row r="11" spans="1:22" x14ac:dyDescent="0.35">
       <c r="B11">
         <f t="shared" si="7"/>
-        <v>-40.309292500000005</v>
+        <v>20.149515250000015</v>
       </c>
       <c r="C11">
         <f t="shared" si="8"/>
@@ -1681,7 +1695,7 @@
       </c>
       <c r="D11">
         <f t="shared" si="9"/>
-        <v>-40.188692500000002</v>
+        <v>20.270115250000014</v>
       </c>
       <c r="E11">
         <f t="shared" si="10"/>
@@ -1754,7 +1768,7 @@
     <row r="12" spans="1:22" x14ac:dyDescent="0.35">
       <c r="B12">
         <f t="shared" si="7"/>
-        <v>-40.3692925</v>
+        <v>20.089515250000016</v>
       </c>
       <c r="C12">
         <f t="shared" si="8"/>
@@ -1762,7 +1776,7 @@
       </c>
       <c r="D12">
         <f t="shared" si="9"/>
-        <v>-40.309292500000005</v>
+        <v>20.149515250000015</v>
       </c>
       <c r="E12">
         <f t="shared" si="10"/>
@@ -1927,13 +1941,13 @@
     <row r="16" spans="1:22" x14ac:dyDescent="0.35">
       <c r="G16" s="4" t="str">
         <f>LEFT(G4,K4)&amp;TEXT(B4,"#0.0000")&amp;" "&amp;TEXT(C4,"#0.0000")&amp;MID(G4,M4-1,N4-M4+2)&amp;TEXT(D4,"#0.0000")&amp;" "&amp;TEXT(E4,"#0.0000")&amp;RIGHT(G4,LEN(G4)-P4+3)</f>
-        <v xml:space="preserve">  (segment (start -40.2034 119.8426) (end -39.7366 120.26655) (width 0.1524) (layer Front) (net 5))</v>
+        <v xml:space="preserve">  (segment (start 20.2554 119.8426) (end 20.7222 120.26655) (width 0.1524) (layer Front) (net 5))</v>
       </c>
     </row>
     <row r="17" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G17" s="4" t="str">
         <f t="shared" ref="G17:G30" si="16">LEFT(G5,K5)&amp;TEXT(B5,"#0.0000")&amp;" "&amp;TEXT(C5,"#0.0000")&amp;MID(G5,M5-1,N5-M5+2)&amp;TEXT(D5,"#0.0000")&amp;" "&amp;TEXT(E5,"#0.0000")&amp;RIGHT(G5,LEN(G5)-P5+3)</f>
-        <v xml:space="preserve">  (segment (start -40.2034 119.8426) (end -40.6178 120.31777) (width 0.1524) (layer Front) (net 5))</v>
+        <v xml:space="preserve">  (segment (start 20.2554 119.8426) (end 19.8410 120.31777) (width 0.1524) (layer Front) (net 5))</v>
       </c>
     </row>
     <row r="18" spans="7:7" x14ac:dyDescent="0.35">
@@ -1951,31 +1965,31 @@
     <row r="20" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G20" s="4" t="str">
         <f t="shared" si="16"/>
-        <v xml:space="preserve">  (segment (start -41.9756 121.3496) (end -41.9796 121.34877) (width 0.1524) (layer Back) (net 10))</v>
+        <v xml:space="preserve">  (segment (start 18.4832 121.3496) (end 18.4792 121.34877) (width 0.1524) (layer Back) (net 10))</v>
       </c>
     </row>
     <row r="21" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G21" s="4" t="str">
         <f t="shared" si="16"/>
-        <v xml:space="preserve">  (segment (start -40.3693 121.7052) (end -41.9756 121.34966) (width 0.1524) (layer Back) (net 10))</v>
+        <v xml:space="preserve">  (segment (start 20.0895 121.7052) (end 18.4832 121.34966) (width 0.1524) (layer Back) (net 10))</v>
       </c>
     </row>
     <row r="22" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G22" s="4" t="str">
         <f t="shared" si="16"/>
-        <v xml:space="preserve">  (segment (start -40.1887 121.7301) (end -40.1279 121.72866) (width 0.1524) (layer Back) (net 10))</v>
+        <v xml:space="preserve">  (segment (start 20.2701 121.7301) (end 20.3309 121.72866) (width 0.1524) (layer Back) (net 10))</v>
       </c>
     </row>
     <row r="23" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G23" s="4" t="str">
         <f t="shared" si="16"/>
-        <v xml:space="preserve">  (segment (start -40.3093 121.7184) (end -40.1887 121.73011) (width 0.1524) (layer Back) (net 10))</v>
+        <v xml:space="preserve">  (segment (start 20.1495 121.7184) (end 20.2701 121.73011) (width 0.1524) (layer Back) (net 10))</v>
       </c>
     </row>
     <row r="24" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G24" s="4" t="str">
         <f t="shared" si="16"/>
-        <v xml:space="preserve">  (segment (start -40.3693 121.7052) (end -40.3093 121.71844) (width 0.1524) (layer Back) (net 10))</v>
+        <v xml:space="preserve">  (segment (start 20.0895 121.7052) (end 20.1495 121.71844) (width 0.1524) (layer Back) (net 10))</v>
       </c>
     </row>
     <row r="25" spans="7:7" x14ac:dyDescent="0.35">
@@ -2022,9 +2036,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:V8"/>
+  <dimension ref="B1:AD8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
@@ -2049,47 +2063,72 @@
     <col min="19" max="19" width="2.1796875" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="2.36328125" customWidth="1"/>
     <col min="21" max="22" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="1.81640625" customWidth="1"/>
+    <col min="25" max="25" width="4.81640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="2.08984375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.08984375" customWidth="1"/>
+    <col min="28" max="28" width="4.1796875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="2.08984375" customWidth="1"/>
+    <col min="30" max="30" width="2.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:22" ht="10" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="11">
+    <row r="1" spans="2:30" ht="10" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="10">
         <f>B4-B3</f>
-        <v>-31.78</v>
-      </c>
-      <c r="C1" s="11">
+        <v>-52.92</v>
+      </c>
+      <c r="C1" s="10">
         <f>C4-C3</f>
-        <v>33.239000000000004</v>
-      </c>
-      <c r="D1" s="11">
+        <v>1.2390000000000043</v>
+      </c>
+      <c r="D1" s="10">
         <f>D4-D3</f>
         <v>0</v>
       </c>
-      <c r="F1" s="11">
+      <c r="F1" s="10">
         <f>B1</f>
-        <v>-31.78</v>
-      </c>
-      <c r="G1" s="11">
+        <v>-52.92</v>
+      </c>
+      <c r="G1" s="10">
         <f t="shared" ref="G1:H1" si="0">C1</f>
-        <v>33.239000000000004</v>
-      </c>
-      <c r="H1" s="11">
+        <v>1.2390000000000043</v>
+      </c>
+      <c r="H1" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L1" s="12" t="s">
+      <c r="L1" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="N1" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="O1" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y1" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z1" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA1" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB1" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="M1" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="N1" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="O1" s="12" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="AC1" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="AD1" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="2:30" x14ac:dyDescent="0.35">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -2118,81 +2157,88 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:30" x14ac:dyDescent="0.35">
       <c r="B3">
-        <v>144.78</v>
+        <v>121.92</v>
       </c>
       <c r="C3">
         <v>119.761</v>
       </c>
       <c r="D3">
-        <v>270</v>
+        <v>180</v>
       </c>
       <c r="E3" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F3">
         <f>VALUE(MID($K3,L3+LEN(L$1),M3-L3-LEN(L$1)))</f>
-        <v>136.52500000000001</v>
+        <v>116.33199999999999</v>
       </c>
       <c r="G3">
-        <f>VALUE(MID($K3,M3+LEN(M$1),N3-M3-LEN(M$1)))</f>
-        <v>125.98399999999999</v>
+        <f>IFERROR(VALUE(MID($K3,M3+LEN(M$1),N3-M3-LEN(M$1))),VALUE(MID($K3,M3+LEN(M$1),LEN($K3)-M3-1)))</f>
+        <v>126.111</v>
       </c>
       <c r="H3">
-        <f>VALUE(MID($K3,N3+LEN(N$1),O3-N3-LEN(N$1)))</f>
+        <f>IFERROR(VALUE(MID($K3,N3+LEN(N$1),O3-N3-LEN(N$1))),0)</f>
         <v>180</v>
       </c>
       <c r="I3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="K3" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="L3" s="13">
+      <c r="L3" s="12">
         <f>FIND(L$1,$K3)</f>
         <v>6</v>
       </c>
-      <c r="M3" s="13">
+      <c r="M3" s="12">
         <f>FIND(M$1,$K3,L3+LEN(L$1))</f>
         <v>16</v>
       </c>
-      <c r="N3" s="13">
+      <c r="N3" s="12">
         <f>FIND(N$1,$K3,M3+LEN(M$1))</f>
         <v>24</v>
       </c>
-      <c r="O3" s="13">
+      <c r="O3" s="12">
         <f>FIND(O$1,$K3,N3+LEN(N$1))</f>
         <v>28</v>
       </c>
-      <c r="U3" s="10">
-        <v>99.460995999999994</v>
+      <c r="U3">
+        <f>VALUE(MID($X3,Y4+LEN(Y$1),Z4-Y4-LEN(Y$1)))</f>
+        <v>57.467500000000001</v>
       </c>
       <c r="V3">
-        <v>156.21478300000001</v>
-      </c>
-    </row>
-    <row r="4" spans="2:22" x14ac:dyDescent="0.35">
-      <c r="B4">
-        <v>113</v>
-      </c>
-      <c r="C4">
-        <v>153</v>
+        <f>VALUE(MID($X3,Z4+LEN(Z$1),AA4-Z4-LEN(Z$1)))</f>
+        <v>122.91549999999999</v>
+      </c>
+      <c r="X3" s="10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="2:30" x14ac:dyDescent="0.35">
+      <c r="B4" s="13">
+        <f>U8</f>
+        <v>69</v>
+      </c>
+      <c r="C4" s="13">
+        <f>V8</f>
+        <v>121</v>
       </c>
       <c r="D4">
-        <v>270</v>
+        <v>180</v>
       </c>
       <c r="E4" t="str">
         <f>E3&amp;"'"</f>
-        <v>U1'</v>
+        <v>U2'</v>
       </c>
       <c r="F4">
         <f>F3+F1</f>
-        <v>104.745</v>
+        <v>63.411999999999992</v>
       </c>
       <c r="G4">
         <f>G3+G1</f>
-        <v>159.22300000000001</v>
+        <v>127.35000000000001</v>
       </c>
       <c r="H4">
         <f>H3+H1</f>
@@ -2203,40 +2249,97 @@
         <v>R2'</v>
       </c>
       <c r="K4" t="str">
-        <f>LEFT(K3,L3+LEN(L$1)-1)&amp;TEXT(F4,"#0.0####")&amp;" "&amp;TEXT(G4,"#0.0####")&amp;" "&amp;TEXT(H4,"#0")&amp;RIGHT(K3,LEN(K3)-O3+1)</f>
-        <v xml:space="preserve">    (at 104.745 159.223 180)</v>
+        <f>LEFT(K3,L3+LEN(L$1)-1)&amp;TEXT(F4,"#0.0####")&amp;" "&amp;TEXT(G4,"#0.0####")&amp;" "&amp;TEXT(H4,"#0")&amp;O$1</f>
+        <v xml:space="preserve">    (at 63.412 127.35 180)</v>
       </c>
       <c r="U4">
-        <v>96.173552999999998</v>
+        <f>VALUE(MID($X3,AB4+LEN(AB$1),AC4-AB4-LEN(AB$1)))</f>
+        <v>57.467500000000001</v>
       </c>
       <c r="V4">
-        <v>155.92716899999999</v>
-      </c>
-    </row>
-    <row r="5" spans="2:22" x14ac:dyDescent="0.35">
+        <f>VALUE(MID($X3,AC4+LEN(AC$1),AD4-AC4-LEN(AC$1)))</f>
+        <v>119.8145</v>
+      </c>
+      <c r="Y4" s="12">
+        <f>FIND(Y$1,$X3)</f>
+        <v>13</v>
+      </c>
+      <c r="Z4" s="12">
+        <f>FIND(Z$1,$X3,Y4+LEN(Y$1))</f>
+        <v>26</v>
+      </c>
+      <c r="AA4" s="12">
+        <f>FIND(AA$1,$X3,Z4+LEN(Z$1))</f>
+        <v>35</v>
+      </c>
+      <c r="AB4" s="12">
+        <f>FIND(AB$1,$X3)</f>
+        <v>38</v>
+      </c>
+      <c r="AC4" s="12">
+        <f>FIND(AC$1,$X3,AB4+LEN(AB$1))</f>
+        <v>49</v>
+      </c>
+      <c r="AD4" s="12">
+        <f>FIND(AD$1,$X3,AC4+LEN(AC$1))</f>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="2:30" x14ac:dyDescent="0.35">
       <c r="U5">
-        <v>138.15238299999999</v>
+        <f>VALUE(MID($X5,Y6+LEN(Y$1),Z6-Y6-LEN(Y$1)))</f>
+        <v>80.481628000000001</v>
       </c>
       <c r="V5">
-        <v>157.72632999999999</v>
-      </c>
-    </row>
-    <row r="6" spans="2:22" x14ac:dyDescent="0.35">
+        <f>VALUE(MID($X5,Z6+LEN(Z$1),AA6-Z6-LEN(Z$1)))</f>
+        <v>118.59572799999999</v>
+      </c>
+      <c r="X5" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="2:30" x14ac:dyDescent="0.35">
       <c r="U6">
-        <v>137.365522</v>
+        <f>VALUE(MID($X5,AB6+LEN(AB$1),AC6-AB6-LEN(AB$1)))</f>
+        <v>79.976212000000004</v>
       </c>
       <c r="V6">
-        <v>157.86507499999999</v>
-      </c>
-    </row>
-    <row r="8" spans="2:22" x14ac:dyDescent="0.35">
-      <c r="U8" s="10">
+        <f>VALUE(MID($X5,AC6+LEN(AC$1),AD6-AC6-LEN(AC$1)))</f>
+        <v>124.37266200000001</v>
+      </c>
+      <c r="Y6" s="12">
+        <f>FIND(Y$1,$X5)</f>
+        <v>13</v>
+      </c>
+      <c r="Z6" s="12">
+        <f>FIND(Z$1,$X5,Y6+LEN(Y$1))</f>
+        <v>28</v>
+      </c>
+      <c r="AA6" s="12">
+        <f>FIND(AA$1,$X5,Z6+LEN(Z$1))</f>
+        <v>39</v>
+      </c>
+      <c r="AB6" s="12">
+        <f>FIND(AB$1,$X5)</f>
+        <v>42</v>
+      </c>
+      <c r="AC6" s="12">
+        <f>FIND(AC$1,$X5,AB6+LEN(AB$1))</f>
+        <v>55</v>
+      </c>
+      <c r="AD6" s="12">
+        <f>FIND(AD$1,$X5,AC6+LEN(AC$1))</f>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="2:30" x14ac:dyDescent="0.35">
+      <c r="U8" s="13">
         <f>ROUND(AVERAGE(U3:U6),0)</f>
-        <v>118</v>
-      </c>
-      <c r="V8" s="10">
+        <v>69</v>
+      </c>
+      <c r="V8" s="13">
         <f>ROUND(AVERAGE(V3:V6),0)</f>
-        <v>157</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
moved a few edge cuts
</commit_message>
<xml_diff>
--- a/KiCadHacks.xlsx
+++ b/KiCadHacks.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="7200" windowWidth="23720" windowHeight="5180" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="7800" windowWidth="23720" windowHeight="5180" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="MoveSW" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="31">
   <si>
     <t>X</t>
   </si>
@@ -113,6 +113,12 @@
   </si>
   <si>
     <t xml:space="preserve">    (at 38.497 38.615 0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  (gr_line (start 177.828 163.422) (end 177.828 133.026) (angle 90) (layer Edge.Cuts) (width 0.127))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  (gr_line (start 173.751997 128.026049) (end 168.99606 128.027285) (layer Dwgs.User) (width 0.1))</t>
   </si>
 </sst>
 </file>
@@ -1075,8 +1081,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="Y14" sqref="Y14"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14:E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1235,7 +1241,7 @@
         <v>1</v>
       </c>
       <c r="I5" s="1">
-        <f t="shared" ref="I5:V8" si="2">FIND(" ",$G5,H5+1)</f>
+        <f t="shared" ref="I5:V5" si="2">FIND(" ",$G5,H5+1)</f>
         <v>2</v>
       </c>
       <c r="J5" s="1">
@@ -1509,20 +1515,20 @@
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.35">
       <c r="B10">
-        <f t="shared" ref="B10:E10" si="17">B12+ROUND($Z7,2)</f>
-        <v>65.112873999999991</v>
+        <f t="shared" ref="B10:C10" si="17">B12+ROUND($Z7,2)</f>
+        <v>177.37800000000001</v>
       </c>
       <c r="C10">
         <f t="shared" si="17"/>
-        <v>140.06220000000002</v>
+        <v>162.97200000000001</v>
       </c>
       <c r="D10">
         <f>D12+ROUND($Z7,2)</f>
-        <v>65.112872999999993</v>
+        <v>177.37800000000001</v>
       </c>
       <c r="E10">
         <f t="shared" ref="E10" si="18">E12+ROUND($Z7,2)</f>
-        <v>164.65858300000002</v>
+        <v>132.57600000000002</v>
       </c>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
@@ -1568,22 +1574,22 @@
     <row r="12" spans="1:26" x14ac:dyDescent="0.35">
       <c r="B12">
         <f>VALUE(MID($G12,K12,L12-K12))</f>
-        <v>65.562873999999994</v>
+        <v>177.828</v>
       </c>
       <c r="C12">
         <f>VALUE(MID($G12,L12,M12-L12-1))</f>
-        <v>140.51220000000001</v>
+        <v>163.422</v>
       </c>
       <c r="D12">
         <f>VALUE(MID($G12,N12,O12-N12))</f>
-        <v>65.562872999999996</v>
+        <v>177.828</v>
       </c>
       <c r="E12">
         <f>VALUE(MID($G12,O12,P12-O12-1))</f>
-        <v>165.10858300000001</v>
+        <v>133.02600000000001</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="H12" s="1">
         <f t="shared" si="1"/>
@@ -1603,43 +1609,43 @@
       </c>
       <c r="L12" s="1">
         <f t="shared" si="19"/>
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="M12" s="1">
         <f t="shared" si="19"/>
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="N12" s="1">
         <f t="shared" si="19"/>
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="O12" s="1">
         <f t="shared" si="19"/>
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="P12" s="1">
         <f t="shared" si="19"/>
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="Q12" s="1">
         <f t="shared" si="19"/>
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="R12" s="1">
         <f t="shared" si="19"/>
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="S12" s="1">
         <f t="shared" si="19"/>
-        <v>90</v>
-      </c>
-      <c r="T12" s="1" t="e">
+        <v>75</v>
+      </c>
+      <c r="T12" s="1">
         <f t="shared" si="19"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="U12" s="1" t="e">
+        <v>86</v>
+      </c>
+      <c r="U12" s="1">
         <f t="shared" si="19"/>
-        <v>#VALUE!</v>
+        <v>93</v>
       </c>
       <c r="V12" s="1" t="e">
         <f t="shared" si="19"/>
@@ -1655,84 +1661,103 @@
       </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="B13" t="e">
-        <f t="shared" ref="B9:B13" si="20">VALUE(MID($G13,K13,L13-K13))+B$3</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C13" t="e">
-        <f t="shared" ref="C9:C13" si="21">VALUE(MID($G13,L13,M13-L13-1))+C$3</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D13" t="e">
-        <f t="shared" ref="D9:D13" si="22">VALUE(MID($G13,N13,O13-N13))+D$3</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E13" t="e">
-        <f t="shared" ref="E9:E13" si="23">VALUE(MID($G13,O13,P13-O13-1))+E$3</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H13" s="1" t="e">
+      <c r="B13">
+        <f>VALUE(MID($G13,K13,L13-K13))</f>
+        <v>173.75199699999999</v>
+      </c>
+      <c r="C13">
+        <f>VALUE(MID($G13,L13,M13-L13-1))</f>
+        <v>128.026049</v>
+      </c>
+      <c r="D13">
+        <f>VALUE(MID($G13,N13,O13-N13))</f>
+        <v>168.99606</v>
+      </c>
+      <c r="E13">
+        <f>VALUE(MID($G13,O13,P13-O13-1))</f>
+        <v>128.02728500000001</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H13" s="1">
         <f t="shared" si="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I13" s="1" t="e">
-        <f t="shared" ref="I13:V13" si="24">FIND(" ",$G13,H13+1)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="J13" s="1" t="e">
-        <f t="shared" si="24"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K13" s="1" t="e">
-        <f t="shared" si="24"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L13" s="1" t="e">
-        <f t="shared" si="24"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="M13" s="1" t="e">
-        <f t="shared" si="24"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="N13" s="1" t="e">
-        <f t="shared" si="24"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="O13" s="1" t="e">
-        <f t="shared" si="24"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="P13" s="1" t="e">
-        <f t="shared" si="24"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q13" s="1" t="e">
-        <f t="shared" si="24"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="R13" s="1" t="e">
-        <f t="shared" si="24"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="S13" s="1" t="e">
-        <f t="shared" si="24"/>
-        <v>#VALUE!</v>
+        <v>1</v>
+      </c>
+      <c r="I13" s="1">
+        <f t="shared" ref="I13:V13" si="20">FIND(" ",$G13,H13+1)</f>
+        <v>2</v>
+      </c>
+      <c r="J13" s="1">
+        <f t="shared" si="20"/>
+        <v>11</v>
+      </c>
+      <c r="K13" s="1">
+        <f t="shared" si="20"/>
+        <v>18</v>
+      </c>
+      <c r="L13" s="1">
+        <f t="shared" si="20"/>
+        <v>29</v>
+      </c>
+      <c r="M13" s="1">
+        <f t="shared" si="20"/>
+        <v>41</v>
+      </c>
+      <c r="N13" s="1">
+        <f t="shared" si="20"/>
+        <v>46</v>
+      </c>
+      <c r="O13" s="1">
+        <f t="shared" si="20"/>
+        <v>56</v>
+      </c>
+      <c r="P13" s="1">
+        <f t="shared" si="20"/>
+        <v>68</v>
+      </c>
+      <c r="Q13" s="1">
+        <f t="shared" si="20"/>
+        <v>75</v>
+      </c>
+      <c r="R13" s="1">
+        <f t="shared" si="20"/>
+        <v>86</v>
+      </c>
+      <c r="S13" s="1">
+        <f t="shared" si="20"/>
+        <v>93</v>
       </c>
       <c r="T13" s="1" t="e">
-        <f t="shared" si="24"/>
+        <f t="shared" si="20"/>
         <v>#VALUE!</v>
       </c>
       <c r="U13" s="1" t="e">
-        <f t="shared" si="24"/>
+        <f t="shared" si="20"/>
         <v>#VALUE!</v>
       </c>
       <c r="V13" s="1" t="e">
-        <f t="shared" si="24"/>
+        <f t="shared" si="20"/>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="B14">
+        <f>B12</f>
+        <v>177.828</v>
+      </c>
+      <c r="C14">
+        <f>E12</f>
+        <v>133.02600000000001</v>
+      </c>
+      <c r="D14">
+        <f>B14+E14-E12</f>
+        <v>173.279</v>
+      </c>
+      <c r="E14">
+        <f>ROUND(E13-Z7,3)</f>
+        <v>128.477</v>
+      </c>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
@@ -1762,85 +1787,85 @@
     </row>
     <row r="17" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G17" s="4" t="str">
-        <f t="shared" ref="G17:G30" si="25">LEFT(G5,K5)&amp;TEXT(B5,"#0.0000")&amp;" "&amp;TEXT(C5,"#0.0000")&amp;MID(G5,M5-1,N5-M5+2)&amp;TEXT(D5,"#0.0000")&amp;" "&amp;TEXT(E5,"#0.0000")&amp;RIGHT(G5,LEN(G5)-P5+3)</f>
+        <f t="shared" ref="G17:G30" si="21">LEFT(G5,K5)&amp;TEXT(B5,"#0.0000")&amp;" "&amp;TEXT(C5,"#0.0000")&amp;MID(G5,M5-1,N5-M5+2)&amp;TEXT(D5,"#0.0000")&amp;" "&amp;TEXT(E5,"#0.0000")&amp;RIGHT(G5,LEN(G5)-P5+3)</f>
         <v xml:space="preserve">  (gr_line (start 17.6530 29.4640) (end 17.6530 132.20707) (angle 90) (layer Edge.Cuts) (width 0.127))</v>
       </c>
     </row>
     <row r="18" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G18" s="4" t="e">
-        <f t="shared" si="25"/>
+        <f t="shared" si="21"/>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="19" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G19" s="4" t="e">
-        <f t="shared" si="25"/>
+        <f t="shared" si="21"/>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="20" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G20" s="4" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="21"/>
         <v xml:space="preserve">  (gr_line (start 65.5629 140.5122) (end 65.5629 165.10863) (layer Dwgs.User) (width 0.1))</v>
       </c>
     </row>
     <row r="21" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G21" s="4" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="21"/>
         <v xml:space="preserve">  (gr_line (start 17.2184 135.9622) (end 61.0129 135.96222) (layer Dwgs.User) (width 0.1))</v>
       </c>
     </row>
     <row r="22" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G22" s="4" t="e">
-        <f t="shared" si="25"/>
+        <f t="shared" si="21"/>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="23" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G23" s="4" t="e">
-        <f t="shared" si="25"/>
+        <f t="shared" si="21"/>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="24" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G24" s="4" t="str">
-        <f t="shared" si="25"/>
-        <v xml:space="preserve">  (gr_line (start 65.5629 140.5122) (end 65.5629 165.10863) (layer Dwgs.User) (width 0.1))</v>
+        <f t="shared" si="21"/>
+        <v xml:space="preserve">  (gr_line (start 177.8280 163.4220) (end 177.8280 133.02606) (angle 90) (layer Edge.Cuts) (width 0.127))</v>
       </c>
     </row>
     <row r="25" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G25" s="4" t="e">
-        <f t="shared" si="25"/>
-        <v>#VALUE!</v>
+      <c r="G25" s="4" t="str">
+        <f t="shared" si="21"/>
+        <v xml:space="preserve">  (gr_line (start 173.7520 128.0260) (end 168.9961 128.02735) (layer Dwgs.User) (width 0.1))</v>
       </c>
     </row>
     <row r="26" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G26" s="4" t="e">
-        <f t="shared" si="25"/>
+        <f t="shared" si="21"/>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="27" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G27" s="4" t="e">
-        <f t="shared" si="25"/>
+        <f t="shared" si="21"/>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="28" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G28" s="4" t="e">
-        <f t="shared" si="25"/>
+        <f t="shared" si="21"/>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="29" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G29" s="4" t="e">
-        <f t="shared" si="25"/>
+        <f t="shared" si="21"/>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="30" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G30" s="4" t="e">
-        <f t="shared" si="25"/>
+        <f t="shared" si="21"/>
         <v>#VALUE!</v>
       </c>
     </row>

</xml_diff>

<commit_message>
more cut line moves
</commit_message>
<xml_diff>
--- a/KiCadHacks.xlsx
+++ b/KiCadHacks.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18067"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="7800" windowWidth="23720" windowHeight="5180" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="8400" windowWidth="23720" windowHeight="5180" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="MoveSW" sheetId="1" r:id="rId1"/>
@@ -115,19 +115,20 @@
     <t xml:space="preserve">    (at 38.497 38.615 0)</t>
   </si>
   <si>
-    <t xml:space="preserve">  (gr_line (start 177.828 163.422) (end 177.828 133.026) (angle 90) (layer Edge.Cuts) (width 0.127))</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  (gr_line (start 173.751997 128.026049) (end 168.99606 128.027285) (layer Dwgs.User) (width 0.1))</t>
+    <t xml:space="preserve">  (gr_line (start 153.167 36.73) (end 144.533 28.097) (angle 90) (layer Edge.Cuts) (width 0.127))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  (gr_line (start 144.78 27.559) (end 142.113 27.559) (angle 90) (layer Edge.Cuts) (width 0.127))</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.000000"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -215,7 +216,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -242,6 +243,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1079,17 +1081,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z30"/>
+  <dimension ref="A1:Z31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14:E14"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="2" customWidth="1"/>
+    <col min="2" max="2" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.1796875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="1.81640625" customWidth="1"/>
-    <col min="7" max="7" width="65.36328125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="68.36328125" style="1" customWidth="1"/>
     <col min="8" max="9" width="1.6328125" style="1" customWidth="1"/>
     <col min="10" max="10" width="2.453125" style="1" customWidth="1"/>
     <col min="11" max="21" width="2.453125" customWidth="1"/>
@@ -1341,7 +1346,7 @@
         <v>38.615000000000002</v>
       </c>
       <c r="Z7">
-        <v>-0.45</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.35">
@@ -1516,19 +1521,19 @@
     <row r="10" spans="1:26" x14ac:dyDescent="0.35">
       <c r="B10">
         <f t="shared" ref="B10:C10" si="17">B12+ROUND($Z7,2)</f>
-        <v>177.37800000000001</v>
+        <v>145.22999999999999</v>
       </c>
       <c r="C10">
         <f t="shared" si="17"/>
-        <v>162.97200000000001</v>
+        <v>28.009</v>
       </c>
       <c r="D10">
         <f>D12+ROUND($Z7,2)</f>
-        <v>177.37800000000001</v>
+        <v>142.56299999999999</v>
       </c>
       <c r="E10">
         <f t="shared" ref="E10" si="18">E12+ROUND($Z7,2)</f>
-        <v>132.57600000000002</v>
+        <v>28.009</v>
       </c>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
@@ -1574,22 +1579,22 @@
     <row r="12" spans="1:26" x14ac:dyDescent="0.35">
       <c r="B12">
         <f>VALUE(MID($G12,K12,L12-K12))</f>
-        <v>177.828</v>
+        <v>144.78</v>
       </c>
       <c r="C12">
         <f>VALUE(MID($G12,L12,M12-L12-1))</f>
-        <v>163.422</v>
+        <v>27.559000000000001</v>
       </c>
       <c r="D12">
         <f>VALUE(MID($G12,N12,O12-N12))</f>
-        <v>177.828</v>
+        <v>142.113</v>
       </c>
       <c r="E12">
         <f>VALUE(MID($G12,O12,P12-O12-1))</f>
-        <v>133.02600000000001</v>
+        <v>27.559000000000001</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H12" s="1">
         <f t="shared" si="1"/>
@@ -1609,43 +1614,43 @@
       </c>
       <c r="L12" s="1">
         <f t="shared" si="19"/>
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M12" s="1">
         <f t="shared" si="19"/>
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N12" s="1">
         <f t="shared" si="19"/>
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="O12" s="1">
         <f t="shared" si="19"/>
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="P12" s="1">
         <f t="shared" si="19"/>
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="Q12" s="1">
         <f t="shared" si="19"/>
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="R12" s="1">
         <f t="shared" si="19"/>
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="S12" s="1">
         <f t="shared" si="19"/>
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="T12" s="1">
         <f t="shared" si="19"/>
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="U12" s="1">
         <f t="shared" si="19"/>
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="V12" s="1" t="e">
         <f t="shared" si="19"/>
@@ -1663,22 +1668,22 @@
     <row r="13" spans="1:26" x14ac:dyDescent="0.35">
       <c r="B13">
         <f>VALUE(MID($G13,K13,L13-K13))</f>
-        <v>173.75199699999999</v>
+        <v>153.167</v>
       </c>
       <c r="C13">
         <f>VALUE(MID($G13,L13,M13-L13-1))</f>
-        <v>128.026049</v>
+        <v>36.729999999999997</v>
       </c>
       <c r="D13">
         <f>VALUE(MID($G13,N13,O13-N13))</f>
-        <v>168.99606</v>
-      </c>
-      <c r="E13">
+        <v>144.53299999999999</v>
+      </c>
+      <c r="E13" s="14">
         <f>VALUE(MID($G13,O13,P13-O13-1))</f>
-        <v>128.02728500000001</v>
+        <v>28.097000000000001</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H13" s="1">
         <f t="shared" si="1"/>
@@ -1698,43 +1703,43 @@
       </c>
       <c r="L13" s="1">
         <f t="shared" si="20"/>
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="M13" s="1">
         <f t="shared" si="20"/>
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="N13" s="1">
         <f t="shared" si="20"/>
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="O13" s="1">
         <f t="shared" si="20"/>
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="P13" s="1">
         <f t="shared" si="20"/>
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="Q13" s="1">
         <f t="shared" si="20"/>
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="R13" s="1">
         <f t="shared" si="20"/>
-        <v>86</v>
+        <v>65</v>
       </c>
       <c r="S13" s="1">
         <f t="shared" si="20"/>
-        <v>93</v>
-      </c>
-      <c r="T13" s="1" t="e">
+        <v>72</v>
+      </c>
+      <c r="T13" s="1">
         <f t="shared" si="20"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="U13" s="1" t="e">
+        <v>83</v>
+      </c>
+      <c r="U13" s="1">
         <f t="shared" si="20"/>
-        <v>#VALUE!</v>
+        <v>90</v>
       </c>
       <c r="V13" s="1" t="e">
         <f t="shared" si="20"/>
@@ -1743,20 +1748,24 @@
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.35">
       <c r="B14">
-        <f>B12</f>
-        <v>177.828</v>
+        <f>MIN(B13,D13)</f>
+        <v>144.53299999999999</v>
       </c>
       <c r="C14">
-        <f>E12</f>
-        <v>133.02600000000001</v>
+        <f>MIN(C13,E13)</f>
+        <v>28.097000000000001</v>
       </c>
       <c r="D14">
-        <f>B14+E14-E12</f>
-        <v>173.279</v>
+        <f>MIN(B12,D12)</f>
+        <v>142.113</v>
       </c>
       <c r="E14">
-        <f>ROUND(E13-Z7,3)</f>
-        <v>128.477</v>
+        <f>C14</f>
+        <v>28.097000000000001</v>
+      </c>
+      <c r="G14" s="4" t="str">
+        <f>LEFT(G13,K13)&amp;TEXT(B14,"#0.0####")&amp;" "&amp;TEXT(C14,"#0.0####")&amp;MID(G13,M13-1,N13-M13+2)&amp;TEXT(D14,"#0.0####")&amp;" "&amp;TEXT(E14,"#0.0####")&amp;RIGHT(G13,LEN(G13)-P13+2)</f>
+        <v xml:space="preserve">  (gr_line (start 144.533 28.097) (end 142.113 28.097) (angle 90) (layer Edge.Cuts) (width 0.127))</v>
       </c>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
@@ -1779,92 +1788,108 @@
         <v>157.58588</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="G16" s="4" t="str">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="B15">
+        <f>MAX(B13,D13)</f>
+        <v>153.167</v>
+      </c>
+      <c r="C15" s="14">
+        <f>MIN(C13,E13)</f>
+        <v>28.097000000000001</v>
+      </c>
+      <c r="D15">
+        <f>ROUND(MAX(B12,D12)-$Z$7,3)</f>
+        <v>144.33000000000001</v>
+      </c>
+      <c r="E15">
+        <f>ROUND(MAX(C12,E12)+$Z$7,3)</f>
+        <v>28.009</v>
+      </c>
+      <c r="G15" s="4" t="str">
+        <f>LEFT(G14,K13)&amp;TEXT(B15,"#0.0####")&amp;" "&amp;TEXT(C15,"#0.0####")&amp;MID(G14,M13-2,N13-M13+2)&amp;TEXT(D15,"#0.0####")&amp;" "&amp;TEXT(E15,"#0.0####")&amp;RIGHT(G14,LEN(G14)-P13+2)</f>
+        <v xml:space="preserve">  (gr_line (start 153.167 28.09797) (en144.33 28.0097) (angle 90) (layer Edge.Cuts) (width 0.127))</v>
+      </c>
+    </row>
+    <row r="17" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G17" s="4" t="str">
         <f>LEFT(G4,K4)&amp;TEXT(B4,"#0.0000")&amp;" "&amp;TEXT(C4,"#0.0000")&amp;MID(G4,M4-1,N4-M4+2)&amp;TEXT(D4,"#0.0000")&amp;" "&amp;TEXT(E4,"#0.0000")&amp;RIGHT(G4,LEN(G4)-P4+3)</f>
         <v xml:space="preserve">  (gr_line (start 17.2184 35.7651) (end 17.2184 135.96222) (layer Dwgs.User) (width 0.1))</v>
       </c>
     </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G17" s="4" t="str">
-        <f t="shared" ref="G17:G30" si="21">LEFT(G5,K5)&amp;TEXT(B5,"#0.0000")&amp;" "&amp;TEXT(C5,"#0.0000")&amp;MID(G5,M5-1,N5-M5+2)&amp;TEXT(D5,"#0.0000")&amp;" "&amp;TEXT(E5,"#0.0000")&amp;RIGHT(G5,LEN(G5)-P5+3)</f>
+    <row r="18" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G18" s="4" t="str">
+        <f>LEFT(G5,K5)&amp;TEXT(B5,"#0.0000")&amp;" "&amp;TEXT(C5,"#0.0000")&amp;MID(G5,M5-1,N5-M5+2)&amp;TEXT(D5,"#0.0000")&amp;" "&amp;TEXT(E5,"#0.0000")&amp;RIGHT(G5,LEN(G5)-P5+3)</f>
         <v xml:space="preserve">  (gr_line (start 17.6530 29.4640) (end 17.6530 132.20707) (angle 90) (layer Edge.Cuts) (width 0.127))</v>
-      </c>
-    </row>
-    <row r="18" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G18" s="4" t="e">
-        <f t="shared" si="21"/>
-        <v>#VALUE!</v>
       </c>
     </row>
     <row r="19" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G19" s="4" t="e">
-        <f t="shared" si="21"/>
+        <f>LEFT(G6,K6)&amp;TEXT(B6,"#0.0000")&amp;" "&amp;TEXT(C6,"#0.0000")&amp;MID(G6,M6-1,N6-M6+2)&amp;TEXT(D6,"#0.0000")&amp;" "&amp;TEXT(E6,"#0.0000")&amp;RIGHT(G6,LEN(G6)-P6+3)</f>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="20" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G20" s="4" t="str">
-        <f t="shared" si="21"/>
-        <v xml:space="preserve">  (gr_line (start 65.5629 140.5122) (end 65.5629 165.10863) (layer Dwgs.User) (width 0.1))</v>
+      <c r="G20" s="4" t="e">
+        <f>LEFT(G7,K7)&amp;TEXT(B7,"#0.0000")&amp;" "&amp;TEXT(C7,"#0.0000")&amp;MID(G7,M7-1,N7-M7+2)&amp;TEXT(D7,"#0.0000")&amp;" "&amp;TEXT(E7,"#0.0000")&amp;RIGHT(G7,LEN(G7)-P7+3)</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="21" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G21" s="4" t="str">
-        <f t="shared" si="21"/>
+        <f>LEFT(G8,K8)&amp;TEXT(B8,"#0.0000")&amp;" "&amp;TEXT(C8,"#0.0000")&amp;MID(G8,M8-1,N8-M8+2)&amp;TEXT(D8,"#0.0000")&amp;" "&amp;TEXT(E8,"#0.0000")&amp;RIGHT(G8,LEN(G8)-P8+3)</f>
+        <v xml:space="preserve">  (gr_line (start 65.5629 140.5122) (end 65.5629 165.10863) (layer Dwgs.User) (width 0.1))</v>
+      </c>
+    </row>
+    <row r="22" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G22" s="4" t="str">
+        <f>LEFT(G9,K9)&amp;TEXT(B9,"#0.0000")&amp;" "&amp;TEXT(C9,"#0.0000")&amp;MID(G9,M9-1,N9-M9+2)&amp;TEXT(D9,"#0.0000")&amp;" "&amp;TEXT(E9,"#0.0000")&amp;RIGHT(G9,LEN(G9)-P9+3)</f>
         <v xml:space="preserve">  (gr_line (start 17.2184 135.9622) (end 61.0129 135.96222) (layer Dwgs.User) (width 0.1))</v>
-      </c>
-    </row>
-    <row r="22" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G22" s="4" t="e">
-        <f t="shared" si="21"/>
-        <v>#VALUE!</v>
       </c>
     </row>
     <row r="23" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G23" s="4" t="e">
-        <f t="shared" si="21"/>
+        <f>LEFT(G10,K10)&amp;TEXT(B10,"#0.0000")&amp;" "&amp;TEXT(C10,"#0.0000")&amp;MID(G10,M10-1,N10-M10+2)&amp;TEXT(D10,"#0.0000")&amp;" "&amp;TEXT(E10,"#0.0000")&amp;RIGHT(G10,LEN(G10)-P10+3)</f>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="24" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G24" s="4" t="str">
-        <f t="shared" si="21"/>
-        <v xml:space="preserve">  (gr_line (start 177.8280 163.4220) (end 177.8280 133.02606) (angle 90) (layer Edge.Cuts) (width 0.127))</v>
+      <c r="G24" s="4" t="e">
+        <f>LEFT(G11,K11)&amp;TEXT(B11,"#0.0000")&amp;" "&amp;TEXT(C11,"#0.0000")&amp;MID(G11,M11-1,N11-M11+2)&amp;TEXT(D11,"#0.0000")&amp;" "&amp;TEXT(E11,"#0.0000")&amp;RIGHT(G11,LEN(G11)-P11+3)</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="25" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G25" s="4" t="str">
-        <f t="shared" si="21"/>
-        <v xml:space="preserve">  (gr_line (start 173.7520 128.0260) (end 168.9961 128.02735) (layer Dwgs.User) (width 0.1))</v>
-      </c>
-    </row>
-    <row r="26" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G26" s="4" t="e">
-        <f t="shared" si="21"/>
-        <v>#VALUE!</v>
+        <f>LEFT(G12,K12)&amp;TEXT(B12,"#0.0000")&amp;" "&amp;TEXT(C12,"#0.0000")&amp;MID(G12,M12-1,N12-M12+2)&amp;TEXT(D12,"#0.0000")&amp;" "&amp;TEXT(E12,"#0.0000")&amp;RIGHT(G12,LEN(G12)-P12+3)</f>
+        <v xml:space="preserve">  (gr_line (start 144.7800 27.5590) (end 142.1130 27.55909) (angle 90) (layer Edge.Cuts) (width 0.127))</v>
       </c>
     </row>
     <row r="27" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G27" s="4" t="e">
-        <f t="shared" si="21"/>
-        <v>#VALUE!</v>
+        <f>LEFT(#REF!,K14)&amp;TEXT(B14,"#0.0000")&amp;" "&amp;TEXT(C14,"#0.0000")&amp;MID(#REF!,M14-1,N14-M14+2)&amp;TEXT(D14,"#0.0000")&amp;" "&amp;TEXT(E14,"#0.0000")&amp;RIGHT(#REF!,LEN(#REF!)-P14+3)</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="28" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G28" s="4" t="e">
-        <f t="shared" si="21"/>
+        <f>LEFT(G15,K15)&amp;TEXT(B15,"#0.0000")&amp;" "&amp;TEXT(C15,"#0.0000")&amp;MID(G15,M15-1,N15-M15+2)&amp;TEXT(D15,"#0.0000")&amp;" "&amp;TEXT(E15,"#0.0000")&amp;RIGHT(G15,LEN(G15)-P15+3)</f>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="29" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G29" s="4" t="e">
-        <f t="shared" si="21"/>
+        <f t="shared" ref="G29:G31" si="21">LEFT(G17,K17)&amp;TEXT(B17,"#0.0000")&amp;" "&amp;TEXT(C17,"#0.0000")&amp;MID(G17,M17-1,N17-M17+2)&amp;TEXT(D17,"#0.0000")&amp;" "&amp;TEXT(E17,"#0.0000")&amp;RIGHT(G17,LEN(G17)-P17+3)</f>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="30" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G30" s="4" t="e">
+        <f t="shared" si="21"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="31" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G31" s="4" t="e">
         <f t="shared" si="21"/>
         <v>#VALUE!</v>
       </c>

</xml_diff>

<commit_message>
finished edge cut lines
</commit_message>
<xml_diff>
--- a/KiCadHacks.xlsx
+++ b/KiCadHacks.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="8400" windowWidth="23720" windowHeight="5180" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="9000" windowWidth="23720" windowHeight="5180" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="MoveSW" sheetId="1" r:id="rId1"/>
@@ -115,10 +115,10 @@
     <t xml:space="preserve">    (at 38.497 38.615 0)</t>
   </si>
   <si>
-    <t xml:space="preserve">  (gr_line (start 153.167 36.73) (end 144.533 28.097) (angle 90) (layer Edge.Cuts) (width 0.127))</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  (gr_line (start 144.78 27.559) (end 142.113 27.559) (angle 90) (layer Edge.Cuts) (width 0.127))</t>
+    <t xml:space="preserve">  (gr_line (start 65.562873 165.108583) (end 70.112873 169.658583) (layer Dwgs.User) (width 0.1))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  (gr_line (start 66.013 168.527) (end 95.0 170.815) (angle 90) (layer Edge.Cuts) (width 0.127))</t>
   </si>
 </sst>
 </file>
@@ -1081,7 +1081,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z31"/>
+  <dimension ref="A1:AA31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
@@ -1099,10 +1099,12 @@
     <col min="10" max="10" width="2.453125" style="1" customWidth="1"/>
     <col min="11" max="21" width="2.453125" customWidth="1"/>
     <col min="22" max="22" width="6.6328125" customWidth="1"/>
+    <col min="26" max="26" width="4.81640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="8.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:27" ht="8.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.35">
       <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
@@ -1116,7 +1118,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -1140,7 +1142,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.35">
       <c r="B4">
         <f>VALUE(MID($G4,K4,L4-K4))</f>
         <v>17.218363</v>
@@ -1221,7 +1223,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.35">
       <c r="B5">
         <f>VALUE(MID($G5,K5,L5-K5))</f>
         <v>17.652999999999999</v>
@@ -1302,7 +1304,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.35">
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
@@ -1316,7 +1318,7 @@
       <c r="U6" s="1"/>
       <c r="V6" s="1"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
@@ -1348,8 +1350,11 @@
       <c r="Z7">
         <v>0.45</v>
       </c>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="AA7">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.35">
       <c r="B8">
         <f>VALUE(MID($G8,K8,L8-K8))</f>
         <v>65.562873999999994</v>
@@ -1436,8 +1441,14 @@
       <c r="Y8">
         <v>27.559000000000001</v>
       </c>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="Z8">
+        <v>45</v>
+      </c>
+      <c r="AA8">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.35">
       <c r="B9">
         <f>VALUE(MID($G9,K9,L9-K9))</f>
         <v>17.218363</v>
@@ -1518,22 +1529,22 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.35">
       <c r="B10">
         <f t="shared" ref="B10:C10" si="17">B12+ROUND($Z7,2)</f>
-        <v>145.22999999999999</v>
+        <v>66.012872999999999</v>
       </c>
       <c r="C10">
         <f t="shared" si="17"/>
-        <v>28.009</v>
+        <v>165.558583</v>
       </c>
       <c r="D10">
         <f>D12+ROUND($Z7,2)</f>
-        <v>142.56299999999999</v>
+        <v>70.562872999999996</v>
       </c>
       <c r="E10">
         <f t="shared" ref="E10" si="18">E12+ROUND($Z7,2)</f>
-        <v>28.009</v>
+        <v>170.10858299999998</v>
       </c>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
@@ -1555,7 +1566,7 @@
         <v>156.38604900000001</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.35">
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
@@ -1576,25 +1587,25 @@
         <v>181.95604900000001</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.35">
       <c r="B12">
         <f>VALUE(MID($G12,K12,L12-K12))</f>
-        <v>144.78</v>
+        <v>65.562872999999996</v>
       </c>
       <c r="C12">
         <f>VALUE(MID($G12,L12,M12-L12-1))</f>
-        <v>27.559000000000001</v>
+        <v>165.10858300000001</v>
       </c>
       <c r="D12">
         <f>VALUE(MID($G12,N12,O12-N12))</f>
-        <v>142.113</v>
+        <v>70.112872999999993</v>
       </c>
       <c r="E12">
         <f>VALUE(MID($G12,O12,P12-O12-1))</f>
-        <v>27.559000000000001</v>
+        <v>169.65858299999999</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H12" s="1">
         <f t="shared" si="1"/>
@@ -1614,43 +1625,43 @@
       </c>
       <c r="L12" s="1">
         <f t="shared" si="19"/>
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="M12" s="1">
         <f t="shared" si="19"/>
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="N12" s="1">
         <f t="shared" si="19"/>
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="O12" s="1">
         <f t="shared" si="19"/>
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="P12" s="1">
         <f t="shared" si="19"/>
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="Q12" s="1">
         <f t="shared" si="19"/>
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="R12" s="1">
         <f t="shared" si="19"/>
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="S12" s="1">
         <f t="shared" si="19"/>
-        <v>72</v>
-      </c>
-      <c r="T12" s="1">
+        <v>92</v>
+      </c>
+      <c r="T12" s="1" t="e">
         <f t="shared" si="19"/>
-        <v>83</v>
-      </c>
-      <c r="U12" s="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="U12" s="1" t="e">
         <f t="shared" si="19"/>
-        <v>90</v>
+        <v>#VALUE!</v>
       </c>
       <c r="V12" s="1" t="e">
         <f t="shared" si="19"/>
@@ -1665,25 +1676,25 @@
         <v>25.569999999999993</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.35">
       <c r="B13">
         <f>VALUE(MID($G13,K13,L13-K13))</f>
-        <v>153.167</v>
+        <v>66.013000000000005</v>
       </c>
       <c r="C13">
         <f>VALUE(MID($G13,L13,M13-L13-1))</f>
-        <v>36.729999999999997</v>
+        <v>168.52699999999999</v>
       </c>
       <c r="D13">
         <f>VALUE(MID($G13,N13,O13-N13))</f>
-        <v>144.53299999999999</v>
+        <v>95</v>
       </c>
       <c r="E13" s="14">
         <f>VALUE(MID($G13,O13,P13-O13-1))</f>
-        <v>28.097000000000001</v>
+        <v>170.815</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H13" s="1">
         <f t="shared" si="1"/>
@@ -1703,69 +1714,68 @@
       </c>
       <c r="L13" s="1">
         <f t="shared" si="20"/>
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M13" s="1">
         <f t="shared" si="20"/>
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="N13" s="1">
         <f t="shared" si="20"/>
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="O13" s="1">
         <f t="shared" si="20"/>
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="P13" s="1">
         <f t="shared" si="20"/>
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Q13" s="1">
         <f t="shared" si="20"/>
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="R13" s="1">
         <f t="shared" si="20"/>
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="S13" s="1">
         <f t="shared" si="20"/>
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="T13" s="1">
         <f t="shared" si="20"/>
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="U13" s="1">
         <f t="shared" si="20"/>
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="V13" s="1" t="e">
         <f t="shared" si="20"/>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.35">
       <c r="B14">
-        <f>MIN(B13,D13)</f>
-        <v>144.53299999999999</v>
-      </c>
-      <c r="C14">
-        <f>MIN(C13,E13)</f>
-        <v>28.097000000000001</v>
+        <f>ROUND(MIN(B13,D13),3)</f>
+        <v>66.013000000000005</v>
+      </c>
+      <c r="C14" s="14">
+        <v>164.65899999999999</v>
       </c>
       <c r="D14">
-        <f>MIN(B12,D12)</f>
-        <v>142.113</v>
+        <f>MIN(B13,D13)+ROUND(COS(RADIANS($Z$8))*(SQRT(POWER($B12-$D12,2)+POWER($C12-$E12,2)-$Z$7*$AA$7)),3)</f>
+        <v>70.203000000000003</v>
       </c>
       <c r="E14">
-        <f>C14</f>
-        <v>28.097000000000001</v>
+        <f>C14+ROUND(SIN(RADIANS($Z$8))*SQRT(POWER($B12-$D12,2)+POWER($C12-$E12,2)-$Z$7*$AA$7),3)</f>
+        <v>168.84899999999999</v>
       </c>
       <c r="G14" s="4" t="str">
         <f>LEFT(G13,K13)&amp;TEXT(B14,"#0.0####")&amp;" "&amp;TEXT(C14,"#0.0####")&amp;MID(G13,M13-1,N13-M13+2)&amp;TEXT(D14,"#0.0####")&amp;" "&amp;TEXT(E14,"#0.0####")&amp;RIGHT(G13,LEN(G13)-P13+2)</f>
-        <v xml:space="preserve">  (gr_line (start 144.533 28.097) (end 142.113 28.097) (angle 90) (layer Edge.Cuts) (width 0.127))</v>
+        <v xml:space="preserve">  (gr_line (start 66.013 164.659) (end 70.203 168.849) (angle 90) (layer Edge.Cuts) (width 0.127))</v>
       </c>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
@@ -1779,89 +1789,81 @@
       <c r="T14" s="1"/>
       <c r="U14" s="1"/>
       <c r="V14" s="1"/>
-      <c r="X14">
-        <f>(Y12-X12)*AVERAGE(1/2,1/3)</f>
-        <v>0.52916666666666345</v>
-      </c>
-      <c r="Y14">
-        <f>ROUND(X8-X14,5)</f>
-        <v>157.58588</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.35">
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.35">
       <c r="B15">
-        <f>MAX(B13,D13)</f>
-        <v>153.167</v>
-      </c>
-      <c r="C15" s="14">
-        <f>MIN(C13,E13)</f>
-        <v>28.097000000000001</v>
-      </c>
-      <c r="D15">
-        <f>ROUND(MAX(B12,D12)-$Z$7,3)</f>
-        <v>144.33000000000001</v>
-      </c>
-      <c r="E15">
+        <f>ROUND(MAX(B12,D12)+$Z$7,3)</f>
+        <v>70.563000000000002</v>
+      </c>
+      <c r="C15">
+        <f>C13</f>
+        <v>168.52699999999999</v>
+      </c>
+      <c r="D15" s="14">
+        <f>ROUND(MIN(B12,D12)+$Z$7,3)</f>
+        <v>66.013000000000005</v>
+      </c>
+      <c r="E15" s="14">
         <f>ROUND(MAX(C12,E12)+$Z$7,3)</f>
-        <v>28.009</v>
+        <v>170.10900000000001</v>
       </c>
       <c r="G15" s="4" t="str">
         <f>LEFT(G14,K13)&amp;TEXT(B15,"#0.0####")&amp;" "&amp;TEXT(C15,"#0.0####")&amp;MID(G14,M13-2,N13-M13+2)&amp;TEXT(D15,"#0.0####")&amp;" "&amp;TEXT(E15,"#0.0####")&amp;RIGHT(G14,LEN(G14)-P13+2)</f>
-        <v xml:space="preserve">  (gr_line (start 153.167 28.09797) (en144.33 28.0097) (angle 90) (layer Edge.Cuts) (width 0.127))</v>
+        <v xml:space="preserve">  (gr_line (start 70.563 168.5279) (end66.013 170.10949) (angle 90) (layer Edge.Cuts) (width 0.127))</v>
       </c>
     </row>
     <row r="17" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G17" s="4" t="str">
-        <f>LEFT(G4,K4)&amp;TEXT(B4,"#0.0000")&amp;" "&amp;TEXT(C4,"#0.0000")&amp;MID(G4,M4-1,N4-M4+2)&amp;TEXT(D4,"#0.0000")&amp;" "&amp;TEXT(E4,"#0.0000")&amp;RIGHT(G4,LEN(G4)-P4+3)</f>
+        <f t="shared" ref="G17:G25" si="21">LEFT(G4,K4)&amp;TEXT(B4,"#0.0000")&amp;" "&amp;TEXT(C4,"#0.0000")&amp;MID(G4,M4-1,N4-M4+2)&amp;TEXT(D4,"#0.0000")&amp;" "&amp;TEXT(E4,"#0.0000")&amp;RIGHT(G4,LEN(G4)-P4+3)</f>
         <v xml:space="preserve">  (gr_line (start 17.2184 35.7651) (end 17.2184 135.96222) (layer Dwgs.User) (width 0.1))</v>
       </c>
     </row>
     <row r="18" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G18" s="4" t="str">
-        <f>LEFT(G5,K5)&amp;TEXT(B5,"#0.0000")&amp;" "&amp;TEXT(C5,"#0.0000")&amp;MID(G5,M5-1,N5-M5+2)&amp;TEXT(D5,"#0.0000")&amp;" "&amp;TEXT(E5,"#0.0000")&amp;RIGHT(G5,LEN(G5)-P5+3)</f>
+        <f t="shared" si="21"/>
         <v xml:space="preserve">  (gr_line (start 17.6530 29.4640) (end 17.6530 132.20707) (angle 90) (layer Edge.Cuts) (width 0.127))</v>
       </c>
     </row>
     <row r="19" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G19" s="4" t="e">
-        <f>LEFT(G6,K6)&amp;TEXT(B6,"#0.0000")&amp;" "&amp;TEXT(C6,"#0.0000")&amp;MID(G6,M6-1,N6-M6+2)&amp;TEXT(D6,"#0.0000")&amp;" "&amp;TEXT(E6,"#0.0000")&amp;RIGHT(G6,LEN(G6)-P6+3)</f>
+        <f t="shared" si="21"/>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="20" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G20" s="4" t="e">
-        <f>LEFT(G7,K7)&amp;TEXT(B7,"#0.0000")&amp;" "&amp;TEXT(C7,"#0.0000")&amp;MID(G7,M7-1,N7-M7+2)&amp;TEXT(D7,"#0.0000")&amp;" "&amp;TEXT(E7,"#0.0000")&amp;RIGHT(G7,LEN(G7)-P7+3)</f>
+        <f t="shared" si="21"/>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="21" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G21" s="4" t="str">
-        <f>LEFT(G8,K8)&amp;TEXT(B8,"#0.0000")&amp;" "&amp;TEXT(C8,"#0.0000")&amp;MID(G8,M8-1,N8-M8+2)&amp;TEXT(D8,"#0.0000")&amp;" "&amp;TEXT(E8,"#0.0000")&amp;RIGHT(G8,LEN(G8)-P8+3)</f>
+        <f t="shared" si="21"/>
         <v xml:space="preserve">  (gr_line (start 65.5629 140.5122) (end 65.5629 165.10863) (layer Dwgs.User) (width 0.1))</v>
       </c>
     </row>
     <row r="22" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G22" s="4" t="str">
-        <f>LEFT(G9,K9)&amp;TEXT(B9,"#0.0000")&amp;" "&amp;TEXT(C9,"#0.0000")&amp;MID(G9,M9-1,N9-M9+2)&amp;TEXT(D9,"#0.0000")&amp;" "&amp;TEXT(E9,"#0.0000")&amp;RIGHT(G9,LEN(G9)-P9+3)</f>
+        <f t="shared" si="21"/>
         <v xml:space="preserve">  (gr_line (start 17.2184 135.9622) (end 61.0129 135.96222) (layer Dwgs.User) (width 0.1))</v>
       </c>
     </row>
     <row r="23" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G23" s="4" t="e">
-        <f>LEFT(G10,K10)&amp;TEXT(B10,"#0.0000")&amp;" "&amp;TEXT(C10,"#0.0000")&amp;MID(G10,M10-1,N10-M10+2)&amp;TEXT(D10,"#0.0000")&amp;" "&amp;TEXT(E10,"#0.0000")&amp;RIGHT(G10,LEN(G10)-P10+3)</f>
+        <f t="shared" si="21"/>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="24" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G24" s="4" t="e">
-        <f>LEFT(G11,K11)&amp;TEXT(B11,"#0.0000")&amp;" "&amp;TEXT(C11,"#0.0000")&amp;MID(G11,M11-1,N11-M11+2)&amp;TEXT(D11,"#0.0000")&amp;" "&amp;TEXT(E11,"#0.0000")&amp;RIGHT(G11,LEN(G11)-P11+3)</f>
+        <f t="shared" si="21"/>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="25" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G25" s="4" t="str">
-        <f>LEFT(G12,K12)&amp;TEXT(B12,"#0.0000")&amp;" "&amp;TEXT(C12,"#0.0000")&amp;MID(G12,M12-1,N12-M12+2)&amp;TEXT(D12,"#0.0000")&amp;" "&amp;TEXT(E12,"#0.0000")&amp;RIGHT(G12,LEN(G12)-P12+3)</f>
-        <v xml:space="preserve">  (gr_line (start 144.7800 27.5590) (end 142.1130 27.55909) (angle 90) (layer Edge.Cuts) (width 0.127))</v>
+        <f t="shared" si="21"/>
+        <v xml:space="preserve">  (gr_line (start 65.5629 165.1086) (end 70.1129 169.65863) (layer Dwgs.User) (width 0.1))</v>
       </c>
     </row>
     <row r="27" spans="7:7" x14ac:dyDescent="0.35">
@@ -1878,19 +1880,19 @@
     </row>
     <row r="29" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G29" s="4" t="e">
-        <f t="shared" ref="G29:G31" si="21">LEFT(G17,K17)&amp;TEXT(B17,"#0.0000")&amp;" "&amp;TEXT(C17,"#0.0000")&amp;MID(G17,M17-1,N17-M17+2)&amp;TEXT(D17,"#0.0000")&amp;" "&amp;TEXT(E17,"#0.0000")&amp;RIGHT(G17,LEN(G17)-P17+3)</f>
+        <f t="shared" ref="G29:G31" si="22">LEFT(G17,K17)&amp;TEXT(B17,"#0.0000")&amp;" "&amp;TEXT(C17,"#0.0000")&amp;MID(G17,M17-1,N17-M17+2)&amp;TEXT(D17,"#0.0000")&amp;" "&amp;TEXT(E17,"#0.0000")&amp;RIGHT(G17,LEN(G17)-P17+3)</f>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="30" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G30" s="4" t="e">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="31" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G31" s="4" t="e">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>#VALUE!</v>
       </c>
     </row>

</xml_diff>

<commit_message>
moved trace to R13
</commit_message>
<xml_diff>
--- a/KiCadHacks.xlsx
+++ b/KiCadHacks.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="9000" windowWidth="23720" windowHeight="5180" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="9600" windowWidth="23720" windowHeight="5180" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="MoveSW" sheetId="1" r:id="rId1"/>
     <sheet name="MoveSegments" sheetId="2" r:id="rId2"/>
     <sheet name="MoveMPU" sheetId="3" r:id="rId3"/>
+    <sheet name="MoveLCD" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="36">
   <si>
     <t>X</t>
   </si>
@@ -119,6 +120,21 @@
   </si>
   <si>
     <t xml:space="preserve">  (gr_line (start 66.013 168.527) (end 95.0 170.815) (angle 90) (layer Edge.Cuts) (width 0.127))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    (at 157.58588 103.96079 270)</t>
+  </si>
+  <si>
+    <t>LCD1</t>
+  </si>
+  <si>
+    <t>LCD1'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    (at 38.497 38.615)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  (segment (start 24.227 40.297) (end 24.257 40.521) (width 0.1524) (layer Back) (net 89))</t>
   </si>
 </sst>
 </file>
@@ -130,7 +146,7 @@
     <numFmt numFmtId="165" formatCode="0.000000"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -180,6 +196,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1" tint="0.34998626667073579"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -216,7 +246,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -244,6 +274,10 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1083,7 +1117,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
@@ -2214,4 +2248,345 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:V10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P7" sqref="P7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="1.7265625" customWidth="1"/>
+    <col min="2" max="3" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.81640625" customWidth="1"/>
+    <col min="5" max="5" width="5.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="1.81640625" customWidth="1"/>
+    <col min="7" max="7" width="21.6328125" customWidth="1"/>
+    <col min="8" max="8" width="2.81640625" customWidth="1"/>
+    <col min="9" max="9" width="2.08984375" customWidth="1"/>
+    <col min="10" max="10" width="1.90625" customWidth="1"/>
+    <col min="11" max="11" width="2.08984375" customWidth="1"/>
+    <col min="12" max="12" width="2.36328125" customWidth="1"/>
+    <col min="13" max="13" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="2.26953125" style="16" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="4.81640625" customWidth="1"/>
+    <col min="18" max="19" width="2.08984375" customWidth="1"/>
+    <col min="20" max="20" width="4.1796875" customWidth="1"/>
+    <col min="21" max="22" width="2.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:22" ht="10" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="10">
+        <f>B4-B3</f>
+        <v>119.08888</v>
+      </c>
+      <c r="C1" s="10">
+        <f>C4-C3</f>
+        <v>65.345789999999994</v>
+      </c>
+      <c r="D1" s="10">
+        <f>D4-D3</f>
+        <v>270</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="S1" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="T1" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="U1" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="V1" s="11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="B2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="B3">
+        <f>VALUE(MID($G3,H3+LEN(H$1),I3-H3-LEN(H$1)))</f>
+        <v>38.497</v>
+      </c>
+      <c r="C3">
+        <f>IFERROR(VALUE(MID($G3,I3+LEN(I$1),J3-I3-LEN(I$1))),VALUE(MID($G3,I3+LEN(I$1),LEN($G3)-I3-1)))</f>
+        <v>38.615000000000002</v>
+      </c>
+      <c r="D3">
+        <f>IFERROR(VALUE(MID($G3,J3+LEN(J$1),K3-J3-LEN(J$1))),0)</f>
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="12">
+        <f>FIND(H$1,$G3)</f>
+        <v>6</v>
+      </c>
+      <c r="I3" s="12">
+        <f>FIND(I$1,$G3,H3+LEN(H$1))</f>
+        <v>15</v>
+      </c>
+      <c r="J3" s="12" t="e">
+        <f>FIND(J$1,$G3,I3+LEN(I$1))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K3" s="12" t="e">
+        <f>FIND(K$1,$G3,J3+LEN(J$1))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M3">
+        <f>VALUE(MID($P3,Q4+LEN(Q$1),R4-Q4-LEN(Q$1)))</f>
+        <v>24.227</v>
+      </c>
+      <c r="N3">
+        <f>VALUE(MID($P3,R4+LEN(R$1),S4-R4-LEN(R$1)))</f>
+        <v>40.296999999999997</v>
+      </c>
+      <c r="O3" s="12"/>
+      <c r="P3" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="B4">
+        <f>VALUE(MID($G4,H4+LEN(H$1),I4-H4-LEN(H$1)))</f>
+        <v>157.58588</v>
+      </c>
+      <c r="C4">
+        <f>IFERROR(VALUE(MID($G4,I4+LEN(I$1),J4-I4-LEN(I$1))),VALUE(MID($G4,I4+LEN(I$1),LEN($G4)-I4-1)))</f>
+        <v>103.96079</v>
+      </c>
+      <c r="D4">
+        <f>IFERROR(VALUE(MID($G4,J4+LEN(J$1),K4-J4-LEN(J$1))),0)</f>
+        <v>270</v>
+      </c>
+      <c r="E4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" s="12">
+        <f>FIND(H$1,$G4)</f>
+        <v>6</v>
+      </c>
+      <c r="I4" s="12">
+        <f>FIND(I$1,$G4,H4+LEN(H$1))</f>
+        <v>18</v>
+      </c>
+      <c r="J4" s="12">
+        <f>FIND(J$1,$G4,I4+LEN(I$1))</f>
+        <v>28</v>
+      </c>
+      <c r="K4" s="12">
+        <f>FIND(K$1,$G4,J4+LEN(J$1))</f>
+        <v>32</v>
+      </c>
+      <c r="M4">
+        <f>VALUE(MID($P3,T4+LEN(T$1),U4-T4-LEN(T$1)))</f>
+        <v>24.257000000000001</v>
+      </c>
+      <c r="N4">
+        <f>VALUE(MID($P3,U4+LEN(U$1),V4-U4-LEN(U$1)))</f>
+        <v>40.521000000000001</v>
+      </c>
+      <c r="O4" s="12"/>
+      <c r="Q4" s="12">
+        <f>FIND(Q$1,$P3)</f>
+        <v>13</v>
+      </c>
+      <c r="R4" s="12">
+        <f>FIND(R$1,$P3,Q4+LEN(Q$1))</f>
+        <v>25</v>
+      </c>
+      <c r="S4" s="12">
+        <f>FIND(S$1,$P3,R4+LEN(R$1))</f>
+        <v>32</v>
+      </c>
+      <c r="T4" s="12">
+        <f>FIND(T$1,$P3)</f>
+        <v>35</v>
+      </c>
+      <c r="U4" s="12">
+        <f>FIND(U$1,$P3,T4+LEN(T$1))</f>
+        <v>45</v>
+      </c>
+      <c r="V4" s="12">
+        <f>FIND(V$1,$P3,U4+LEN(U$1))</f>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="B5">
+        <f>VALUE(MID($G5,H5+LEN(H$1),I5-H5-LEN(H$1)))</f>
+        <v>157.58588</v>
+      </c>
+      <c r="C5">
+        <f>IFERROR(VALUE(MID($G5,I5+LEN(I$1),J5-I5-LEN(I$1))),VALUE(MID($G5,I5+LEN(I$1),LEN($G5)-I5-1)))</f>
+        <v>103.96079</v>
+      </c>
+      <c r="D5">
+        <f>IFERROR(VALUE(MID($G5,J5+LEN(J$1),K5-J5-LEN(J$1))),0)</f>
+        <v>270</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="12">
+        <f>FIND(H$1,$G5)</f>
+        <v>6</v>
+      </c>
+      <c r="I5" s="12">
+        <f>FIND(I$1,$G5,H5+LEN(H$1))</f>
+        <v>18</v>
+      </c>
+      <c r="J5" s="12">
+        <f>FIND(J$1,$G5,I5+LEN(I$1))</f>
+        <v>28</v>
+      </c>
+      <c r="K5" s="12">
+        <f>FIND(K$1,$G5,J5+LEN(J$1))</f>
+        <v>32</v>
+      </c>
+      <c r="M5" s="12">
+        <f>M3-B$3</f>
+        <v>-14.27</v>
+      </c>
+      <c r="N5" s="12">
+        <f>N3-C$3</f>
+        <v>1.6819999999999951</v>
+      </c>
+      <c r="O5" s="12"/>
+      <c r="P5" s="15"/>
+    </row>
+    <row r="6" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="B6">
+        <f>B5+B1</f>
+        <v>276.67475999999999</v>
+      </c>
+      <c r="C6">
+        <f>C5+C1</f>
+        <v>169.30658</v>
+      </c>
+      <c r="D6">
+        <f>D5+D1</f>
+        <v>540</v>
+      </c>
+      <c r="E6" t="str">
+        <f>E5&amp;"'"</f>
+        <v>R2'</v>
+      </c>
+      <c r="G6" t="str">
+        <f>LEFT(G5,H5+LEN(H$1)-1)&amp;TEXT(B6,"#0.0####")&amp;" "&amp;TEXT(C6,"#0.0####")&amp;" "&amp;TEXT(D6,"#0")&amp;K$1</f>
+        <v xml:space="preserve">    (at 276.67476 169.30658 540)</v>
+      </c>
+      <c r="M6" s="12">
+        <f>M4-B$3</f>
+        <v>-14.239999999999998</v>
+      </c>
+      <c r="N6" s="12">
+        <f>N4-C$3</f>
+        <v>1.9059999999999988</v>
+      </c>
+      <c r="O6" s="12"/>
+      <c r="Q6" s="12"/>
+      <c r="R6" s="12"/>
+      <c r="S6" s="12"/>
+      <c r="T6" s="12"/>
+      <c r="U6" s="12"/>
+      <c r="V6" s="12"/>
+    </row>
+    <row r="7" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="M7">
+        <f>ROUND(B$4-N5,3)</f>
+        <v>155.904</v>
+      </c>
+      <c r="N7">
+        <f>ROUND(C$4+M5,3)</f>
+        <v>89.691000000000003</v>
+      </c>
+      <c r="P7" t="str">
+        <f>LEFT(P3,Q4+LEN(Q$1)-1)&amp;TEXT(M7,"#0.0####")&amp;" "&amp;TEXT(N7,"#0.0####")&amp;MID(P3,S4,T4-S4+LEN(T$1))&amp;TEXT(M8,"#0.0####")&amp;" "&amp;TEXT(N8,"#0.0####")&amp;RIGHT(P3,LEN(P3)-V4+1)</f>
+        <v xml:space="preserve">  (segment (start 155.904 89.691) (end 155.68 89.721) (width 0.1524) (layer Back) (net 89))</v>
+      </c>
+    </row>
+    <row r="8" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="M8">
+        <f>ROUND(B$4-N6,3)</f>
+        <v>155.68</v>
+      </c>
+      <c r="N8">
+        <f>ROUND(C$4+M6,3)</f>
+        <v>89.721000000000004</v>
+      </c>
+    </row>
+    <row r="9" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="M9" s="12">
+        <f>M3-M4</f>
+        <v>-3.0000000000001137E-2</v>
+      </c>
+      <c r="N9" s="12">
+        <f>N3-N4</f>
+        <v>-0.22400000000000375</v>
+      </c>
+    </row>
+    <row r="10" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="M10" s="12">
+        <f>M7-M8</f>
+        <v>0.22399999999998954</v>
+      </c>
+      <c r="N10" s="12">
+        <f>N7-N8</f>
+        <v>-3.0000000000001137E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
moved LCD components R13, C17, and C16
</commit_message>
<xml_diff>
--- a/KiCadHacks.xlsx
+++ b/KiCadHacks.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="9600" windowWidth="23720" windowHeight="5180" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="10200" windowWidth="23720" windowHeight="5180" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="MoveSW" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="38">
   <si>
     <t>X</t>
   </si>
@@ -134,7 +134,13 @@
     <t xml:space="preserve">    (at 38.497 38.615)</t>
   </si>
   <si>
-    <t xml:space="preserve">  (segment (start 24.227 40.297) (end 24.257 40.521) (width 0.1524) (layer Back) (net 89))</t>
+    <t>C17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    (at 27.94 41.021)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  (segment (start 27.997 39.3979) (end 28.3863 38.9655) (width 0.1524) (layer Back) (net 47))</t>
   </si>
 </sst>
 </file>
@@ -2268,7 +2274,7 @@
     <col min="7" max="7" width="21.6328125" customWidth="1"/>
     <col min="8" max="8" width="2.81640625" customWidth="1"/>
     <col min="9" max="9" width="2.08984375" customWidth="1"/>
-    <col min="10" max="10" width="1.90625" customWidth="1"/>
+    <col min="10" max="10" width="2.54296875" customWidth="1"/>
     <col min="11" max="11" width="2.08984375" customWidth="1"/>
     <col min="12" max="12" width="2.36328125" customWidth="1"/>
     <col min="13" max="13" width="9.81640625" bestFit="1" customWidth="1"/>
@@ -2365,28 +2371,28 @@
         <v>6</v>
       </c>
       <c r="I3" s="12">
-        <f>FIND(I$1,$G3,H3+LEN(H$1))</f>
+        <f t="shared" ref="I3:K5" si="0">FIND(I$1,$G3,H3+LEN(H$1))</f>
         <v>15</v>
       </c>
       <c r="J3" s="12" t="e">
-        <f>FIND(J$1,$G3,I3+LEN(I$1))</f>
+        <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
       <c r="K3" s="12" t="e">
-        <f>FIND(K$1,$G3,J3+LEN(J$1))</f>
+        <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
       <c r="M3">
         <f>VALUE(MID($P3,Q4+LEN(Q$1),R4-Q4-LEN(Q$1)))</f>
-        <v>24.227</v>
+        <v>27.997</v>
       </c>
       <c r="N3">
         <f>VALUE(MID($P3,R4+LEN(R$1),S4-R4-LEN(R$1)))</f>
-        <v>40.296999999999997</v>
+        <v>39.3979</v>
       </c>
       <c r="O3" s="12"/>
       <c r="P3" s="10" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="2:22" x14ac:dyDescent="0.35">
@@ -2413,24 +2419,24 @@
         <v>6</v>
       </c>
       <c r="I4" s="12">
-        <f>FIND(I$1,$G4,H4+LEN(H$1))</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="J4" s="12">
-        <f>FIND(J$1,$G4,I4+LEN(I$1))</f>
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="K4" s="12">
-        <f>FIND(K$1,$G4,J4+LEN(J$1))</f>
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="M4">
         <f>VALUE(MID($P3,T4+LEN(T$1),U4-T4-LEN(T$1)))</f>
-        <v>24.257000000000001</v>
+        <v>28.386299999999999</v>
       </c>
       <c r="N4">
         <f>VALUE(MID($P3,U4+LEN(U$1),V4-U4-LEN(U$1)))</f>
-        <v>40.521000000000001</v>
+        <v>38.965499999999999</v>
       </c>
       <c r="O4" s="12"/>
       <c r="Q4" s="12">
@@ -2443,95 +2449,83 @@
       </c>
       <c r="S4" s="12">
         <f>FIND(S$1,$P3,R4+LEN(R$1))</f>
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="T4" s="12">
         <f>FIND(T$1,$P3)</f>
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="U4" s="12">
         <f>FIND(U$1,$P3,T4+LEN(T$1))</f>
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="V4" s="12">
         <f>FIND(V$1,$P3,U4+LEN(U$1))</f>
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B5">
         <f>VALUE(MID($G5,H5+LEN(H$1),I5-H5-LEN(H$1)))</f>
-        <v>157.58588</v>
+        <v>27.94</v>
       </c>
       <c r="C5">
         <f>IFERROR(VALUE(MID($G5,I5+LEN(I$1),J5-I5-LEN(I$1))),VALUE(MID($G5,I5+LEN(I$1),LEN($G5)-I5-1)))</f>
-        <v>103.96079</v>
+        <v>41.021000000000001</v>
       </c>
       <c r="D5">
         <f>IFERROR(VALUE(MID($G5,J5+LEN(J$1),K5-J5-LEN(J$1))),0)</f>
-        <v>270</v>
+        <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="H5" s="12">
         <f>FIND(H$1,$G5)</f>
         <v>6</v>
       </c>
       <c r="I5" s="12">
-        <f>FIND(I$1,$G5,H5+LEN(H$1))</f>
-        <v>18</v>
-      </c>
-      <c r="J5" s="12">
-        <f>FIND(J$1,$G5,I5+LEN(I$1))</f>
-        <v>28</v>
-      </c>
-      <c r="K5" s="12">
-        <f>FIND(K$1,$G5,J5+LEN(J$1))</f>
-        <v>32</v>
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="J5" s="12" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K5" s="12" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
       </c>
       <c r="M5" s="12">
         <f>M3-B$3</f>
-        <v>-14.27</v>
+        <v>-10.5</v>
       </c>
       <c r="N5" s="12">
         <f>N3-C$3</f>
-        <v>1.6819999999999951</v>
+        <v>0.78289999999999793</v>
       </c>
       <c r="O5" s="12"/>
       <c r="P5" s="15"/>
     </row>
     <row r="6" spans="2:22" x14ac:dyDescent="0.35">
-      <c r="B6">
-        <f>B5+B1</f>
-        <v>276.67475999999999</v>
-      </c>
-      <c r="C6">
-        <f>C5+C1</f>
-        <v>169.30658</v>
-      </c>
-      <c r="D6">
-        <f>D5+D1</f>
-        <v>540</v>
-      </c>
-      <c r="E6" t="str">
-        <f>E5&amp;"'"</f>
-        <v>R2'</v>
-      </c>
-      <c r="G6" t="str">
-        <f>LEFT(G5,H5+LEN(H$1)-1)&amp;TEXT(B6,"#0.0####")&amp;" "&amp;TEXT(C6,"#0.0####")&amp;" "&amp;TEXT(D6,"#0")&amp;K$1</f>
-        <v xml:space="preserve">    (at 276.67476 169.30658 540)</v>
+      <c r="B6" s="12">
+        <f>B5-B3</f>
+        <v>-10.556999999999999</v>
+      </c>
+      <c r="C6" s="12">
+        <f>C5-C3</f>
+        <v>2.4059999999999988</v>
       </c>
       <c r="M6" s="12">
         <f>M4-B$3</f>
-        <v>-14.239999999999998</v>
+        <v>-10.110700000000001</v>
       </c>
       <c r="N6" s="12">
         <f>N4-C$3</f>
-        <v>1.9059999999999988</v>
+        <v>0.3504999999999967</v>
       </c>
       <c r="O6" s="12"/>
       <c r="Q6" s="12"/>
@@ -2542,47 +2536,67 @@
       <c r="V6" s="12"/>
     </row>
     <row r="7" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="B7">
+        <f>ROUND($B$4-C6,3)</f>
+        <v>155.18</v>
+      </c>
+      <c r="C7">
+        <f>ROUND($C$4+B6,3)</f>
+        <v>93.403999999999996</v>
+      </c>
+      <c r="D7">
+        <f>D5+D1</f>
+        <v>270</v>
+      </c>
+      <c r="E7" t="str">
+        <f>E5&amp;"'"</f>
+        <v>C17'</v>
+      </c>
+      <c r="G7" t="str">
+        <f>LEFT(G5,H5+LEN(H$1)-1)&amp;TEXT(B7,"#0.0####")&amp;" "&amp;TEXT(C7,"#0.0####")&amp;" "&amp;TEXT(D7,"#0")&amp;K$1</f>
+        <v xml:space="preserve">    (at 155.18 93.404 270)</v>
+      </c>
       <c r="M7">
-        <f>ROUND(B$4-N5,3)</f>
-        <v>155.904</v>
+        <f>ROUND($B$4-N5,3)</f>
+        <v>156.803</v>
       </c>
       <c r="N7">
-        <f>ROUND(C$4+M5,3)</f>
-        <v>89.691000000000003</v>
+        <f>ROUND($C$4+M5,3)</f>
+        <v>93.460999999999999</v>
       </c>
       <c r="P7" t="str">
         <f>LEFT(P3,Q4+LEN(Q$1)-1)&amp;TEXT(M7,"#0.0####")&amp;" "&amp;TEXT(N7,"#0.0####")&amp;MID(P3,S4,T4-S4+LEN(T$1))&amp;TEXT(M8,"#0.0####")&amp;" "&amp;TEXT(N8,"#0.0####")&amp;RIGHT(P3,LEN(P3)-V4+1)</f>
-        <v xml:space="preserve">  (segment (start 155.904 89.691) (end 155.68 89.721) (width 0.1524) (layer Back) (net 89))</v>
+        <v xml:space="preserve">  (segment (start 156.803 93.461) (end 157.235 93.85) (width 0.1524) (layer Back) (net 47))</v>
       </c>
     </row>
     <row r="8" spans="2:22" x14ac:dyDescent="0.35">
       <c r="M8">
         <f>ROUND(B$4-N6,3)</f>
-        <v>155.68</v>
+        <v>157.23500000000001</v>
       </c>
       <c r="N8">
         <f>ROUND(C$4+M6,3)</f>
-        <v>89.721000000000004</v>
+        <v>93.85</v>
       </c>
     </row>
     <row r="9" spans="2:22" x14ac:dyDescent="0.35">
       <c r="M9" s="12">
         <f>M3-M4</f>
-        <v>-3.0000000000001137E-2</v>
+        <v>-0.38929999999999865</v>
       </c>
       <c r="N9" s="12">
         <f>N3-N4</f>
-        <v>-0.22400000000000375</v>
+        <v>0.43240000000000123</v>
       </c>
     </row>
     <row r="10" spans="2:22" x14ac:dyDescent="0.35">
       <c r="M10" s="12">
         <f>M7-M8</f>
-        <v>0.22399999999998954</v>
+        <v>-0.43200000000001637</v>
       </c>
       <c r="N10" s="12">
         <f>N7-N8</f>
-        <v>-3.0000000000001137E-2</v>
+        <v>-0.38899999999999579</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
moved the rest of the LCD resisters and capaciters
</commit_message>
<xml_diff>
--- a/KiCadHacks.xlsx
+++ b/KiCadHacks.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="10200" windowWidth="23720" windowHeight="5180" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="10800" windowWidth="23720" windowHeight="5180" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="MoveSW" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="40">
   <si>
     <t>X</t>
   </si>
@@ -134,13 +134,19 @@
     <t xml:space="preserve">    (at 38.497 38.615)</t>
   </si>
   <si>
-    <t>C17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    (at 27.94 41.021)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  (segment (start 27.997 39.3979) (end 28.3863 38.9655) (width 0.1524) (layer Back) (net 47))</t>
+    <t>R10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    (at 55.753 41.021 180)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  (segment (start 158.786 121.239) (end 155.98 121.239) (width 0.1524) (layer Back) (net 91))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  (segment (start 55.797 36.665) (end 55.775 37.3388) (width 0.1524) (layer Back) (net 91))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  (segment (start 159.536 121.261) (end 158.862 121.239) (width 0.1524) (layer Back) (net 91))</t>
   </si>
 </sst>
 </file>
@@ -252,7 +258,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -284,6 +290,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2258,10 +2267,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:V10"/>
+  <dimension ref="B1:V16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2384,15 +2393,15 @@
       </c>
       <c r="M3">
         <f>VALUE(MID($P3,Q4+LEN(Q$1),R4-Q4-LEN(Q$1)))</f>
-        <v>27.997</v>
+        <v>55.796999999999997</v>
       </c>
       <c r="N3">
         <f>VALUE(MID($P3,R4+LEN(R$1),S4-R4-LEN(R$1)))</f>
-        <v>39.3979</v>
+        <v>36.664999999999999</v>
       </c>
       <c r="O3" s="12"/>
       <c r="P3" s="10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="2:22" x14ac:dyDescent="0.35">
@@ -2432,11 +2441,11 @@
       </c>
       <c r="M4">
         <f>VALUE(MID($P3,T4+LEN(T$1),U4-T4-LEN(T$1)))</f>
-        <v>28.386299999999999</v>
+        <v>55.774999999999999</v>
       </c>
       <c r="N4">
         <f>VALUE(MID($P3,U4+LEN(U$1),V4-U4-LEN(U$1)))</f>
-        <v>38.965499999999999</v>
+        <v>37.338799999999999</v>
       </c>
       <c r="O4" s="12"/>
       <c r="Q4" s="12">
@@ -2449,25 +2458,25 @@
       </c>
       <c r="S4" s="12">
         <f>FIND(S$1,$P3,R4+LEN(R$1))</f>
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="T4" s="12">
         <f>FIND(T$1,$P3)</f>
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="U4" s="12">
         <f>FIND(U$1,$P3,T4+LEN(T$1))</f>
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="V4" s="12">
         <f>FIND(V$1,$P3,U4+LEN(U$1))</f>
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B5">
         <f>VALUE(MID($G5,H5+LEN(H$1),I5-H5-LEN(H$1)))</f>
-        <v>27.94</v>
+        <v>55.753</v>
       </c>
       <c r="C5">
         <f>IFERROR(VALUE(MID($G5,I5+LEN(I$1),J5-I5-LEN(I$1))),VALUE(MID($G5,I5+LEN(I$1),LEN($G5)-I5-1)))</f>
@@ -2475,12 +2484,12 @@
       </c>
       <c r="D5">
         <f>IFERROR(VALUE(MID($G5,J5+LEN(J$1),K5-J5-LEN(J$1))),0)</f>
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="E5" t="s">
         <v>35</v>
       </c>
-      <c r="G5" s="10" t="s">
+      <c r="G5" s="17" t="s">
         <v>36</v>
       </c>
       <c r="H5" s="12">
@@ -2489,23 +2498,23 @@
       </c>
       <c r="I5" s="12">
         <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="J5" s="12" t="e">
+        <v>15</v>
+      </c>
+      <c r="J5" s="12">
         <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K5" s="12" t="e">
+        <v>22</v>
+      </c>
+      <c r="K5" s="12">
         <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+        <v>26</v>
       </c>
       <c r="M5" s="12">
         <f>M3-B$3</f>
-        <v>-10.5</v>
+        <v>17.299999999999997</v>
       </c>
       <c r="N5" s="12">
         <f>N3-C$3</f>
-        <v>0.78289999999999793</v>
+        <v>-1.9500000000000028</v>
       </c>
       <c r="O5" s="12"/>
       <c r="P5" s="15"/>
@@ -2513,7 +2522,7 @@
     <row r="6" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B6" s="12">
         <f>B5-B3</f>
-        <v>-10.556999999999999</v>
+        <v>17.256</v>
       </c>
       <c r="C6" s="12">
         <f>C5-C3</f>
@@ -2521,11 +2530,11 @@
       </c>
       <c r="M6" s="12">
         <f>M4-B$3</f>
-        <v>-10.110700000000001</v>
+        <v>17.277999999999999</v>
       </c>
       <c r="N6" s="12">
         <f>N4-C$3</f>
-        <v>0.3504999999999967</v>
+        <v>-1.2762000000000029</v>
       </c>
       <c r="O6" s="12"/>
       <c r="Q6" s="12"/>
@@ -2542,61 +2551,195 @@
       </c>
       <c r="C7">
         <f>ROUND($C$4+B6,3)</f>
-        <v>93.403999999999996</v>
+        <v>121.217</v>
       </c>
       <c r="D7">
-        <f>D5+D1</f>
-        <v>270</v>
+        <f>MOD(D5+D1,360)</f>
+        <v>90</v>
       </c>
       <c r="E7" t="str">
         <f>E5&amp;"'"</f>
-        <v>C17'</v>
+        <v>R10'</v>
       </c>
       <c r="G7" t="str">
         <f>LEFT(G5,H5+LEN(H$1)-1)&amp;TEXT(B7,"#0.0####")&amp;" "&amp;TEXT(C7,"#0.0####")&amp;" "&amp;TEXT(D7,"#0")&amp;K$1</f>
-        <v xml:space="preserve">    (at 155.18 93.404 270)</v>
+        <v xml:space="preserve">    (at 155.18 121.217 90)</v>
       </c>
       <c r="M7">
         <f>ROUND($B$4-N5,3)</f>
-        <v>156.803</v>
+        <v>159.536</v>
       </c>
       <c r="N7">
         <f>ROUND($C$4+M5,3)</f>
-        <v>93.460999999999999</v>
+        <v>121.261</v>
       </c>
       <c r="P7" t="str">
         <f>LEFT(P3,Q4+LEN(Q$1)-1)&amp;TEXT(M7,"#0.0####")&amp;" "&amp;TEXT(N7,"#0.0####")&amp;MID(P3,S4,T4-S4+LEN(T$1))&amp;TEXT(M8,"#0.0####")&amp;" "&amp;TEXT(N8,"#0.0####")&amp;RIGHT(P3,LEN(P3)-V4+1)</f>
-        <v xml:space="preserve">  (segment (start 156.803 93.461) (end 157.235 93.85) (width 0.1524) (layer Back) (net 47))</v>
+        <v xml:space="preserve">  (segment (start 159.536 121.261) (end 158.862 121.239) (width 0.1524) (layer Back) (net 91))</v>
       </c>
     </row>
     <row r="8" spans="2:22" x14ac:dyDescent="0.35">
       <c r="M8">
         <f>ROUND(B$4-N6,3)</f>
-        <v>157.23500000000001</v>
+        <v>158.86199999999999</v>
       </c>
       <c r="N8">
         <f>ROUND(C$4+M6,3)</f>
-        <v>93.85</v>
+        <v>121.239</v>
       </c>
     </row>
     <row r="9" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="D9">
+        <f>90+D5</f>
+        <v>270</v>
+      </c>
+      <c r="E9">
+        <f>MOD(D9+D$1,360)</f>
+        <v>180</v>
+      </c>
       <c r="M9" s="12">
         <f>M3-M4</f>
-        <v>-0.38929999999999865</v>
+        <v>2.1999999999998465E-2</v>
       </c>
       <c r="N9" s="12">
         <f>N3-N4</f>
-        <v>0.43240000000000123</v>
+        <v>-0.67379999999999995</v>
       </c>
     </row>
     <row r="10" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="D10">
+        <f>270+D$5</f>
+        <v>450</v>
+      </c>
+      <c r="E10">
+        <f>MOD(D10+D$1,360)</f>
+        <v>0</v>
+      </c>
       <c r="M10" s="12">
         <f>M7-M8</f>
-        <v>-0.43200000000001637</v>
+        <v>0.67400000000000659</v>
       </c>
       <c r="N10" s="12">
         <f>N7-N8</f>
-        <v>-0.38899999999999579</v>
+        <v>2.199999999999136E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="D11">
+        <f>0+D$5</f>
+        <v>180</v>
+      </c>
+      <c r="E11">
+        <f>MOD(D11+D$1,360)</f>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="M12">
+        <f>VALUE(MID($P12,Q13+LEN(Q$1),R13-Q13-LEN(Q$1)))</f>
+        <v>159.536</v>
+      </c>
+      <c r="N12">
+        <f>VALUE(MID($P12,R13+LEN(R$1),S13-R13-LEN(R$1)))</f>
+        <v>121.261</v>
+      </c>
+      <c r="O12" s="12"/>
+      <c r="P12" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="M13">
+        <f>VALUE(MID($P12,T13+LEN(T$1),U13-T13-LEN(T$1)))</f>
+        <v>158.86199999999999</v>
+      </c>
+      <c r="N13">
+        <f>VALUE(MID($P12,U13+LEN(U$1),V13-U13-LEN(U$1)))</f>
+        <v>121.239</v>
+      </c>
+      <c r="O13" s="12"/>
+      <c r="Q13" s="12">
+        <f>FIND(Q$1,$P12)</f>
+        <v>13</v>
+      </c>
+      <c r="R13" s="12">
+        <f>FIND(R$1,$P12,Q13+LEN(Q$1))</f>
+        <v>26</v>
+      </c>
+      <c r="S13" s="12">
+        <f>FIND(S$1,$P12,R13+LEN(R$1))</f>
+        <v>34</v>
+      </c>
+      <c r="T13" s="12">
+        <f>FIND(T$1,$P12)</f>
+        <v>37</v>
+      </c>
+      <c r="U13" s="12">
+        <f>FIND(U$1,$P12,T13+LEN(T$1))</f>
+        <v>48</v>
+      </c>
+      <c r="V13" s="12">
+        <f>FIND(V$1,$P12,U13+LEN(U$1))</f>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="M14" s="12">
+        <f>ROUND(((M12*N13-M13*N12)*(M15-M16)-(M12-M13)*(M15*N16-N15*M16))/((M12-M13)*(N15-N16)-(N12-N13)*(M15-M16)),3)</f>
+        <v>158.86199999999999</v>
+      </c>
+      <c r="N14" s="12">
+        <f>ROUND(((M12*N13-M13*N12)*(N15-N16)-(N12-N13)*(M15*N16-N15*M16))/((M12-M13)*(N15-N16)-(N12-N13)*(M15-M16)),3)</f>
+        <v>121.239</v>
+      </c>
+    </row>
+    <row r="15" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="M15">
+        <f>VALUE(MID($P15,Q16+LEN(Q$1),R16-Q16-LEN(Q$1)))</f>
+        <v>158.786</v>
+      </c>
+      <c r="N15">
+        <f>VALUE(MID($P15,R16+LEN(R$1),S16-R16-LEN(R$1)))</f>
+        <v>121.239</v>
+      </c>
+      <c r="O15" s="12"/>
+      <c r="P15" s="10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="M16">
+        <f>VALUE(MID($P15,T16+LEN(T$1),U16-T16-LEN(T$1)))</f>
+        <v>155.97999999999999</v>
+      </c>
+      <c r="N16">
+        <f>VALUE(MID($P15,U16+LEN(U$1),V16-U16-LEN(U$1)))</f>
+        <v>121.239</v>
+      </c>
+      <c r="O16" s="12"/>
+      <c r="Q16" s="12">
+        <f>FIND(Q$1,$P15)</f>
+        <v>13</v>
+      </c>
+      <c r="R16" s="12">
+        <f>FIND(R$1,$P15,Q16+LEN(Q$1))</f>
+        <v>26</v>
+      </c>
+      <c r="S16" s="12">
+        <f>FIND(S$1,$P15,R16+LEN(R$1))</f>
+        <v>34</v>
+      </c>
+      <c r="T16" s="12">
+        <f>FIND(T$1,$P15)</f>
+        <v>37</v>
+      </c>
+      <c r="U16" s="12">
+        <f>FIND(U$1,$P15,T16+LEN(T$1))</f>
+        <v>47</v>
+      </c>
+      <c r="V16" s="12">
+        <f>FIND(V$1,$P15,U16+LEN(U$1))</f>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
renamed S21 and S22 as the initial switch reorganization step
</commit_message>
<xml_diff>
--- a/KiCadHacks.xlsx
+++ b/KiCadHacks.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="10800" windowWidth="23720" windowHeight="5180" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="11400" windowWidth="23720" windowHeight="5180"/>
   </bookViews>
   <sheets>
     <sheet name="MoveSW" sheetId="1" r:id="rId1"/>
@@ -609,8 +609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -642,7 +642,7 @@
         <v>7</v>
       </c>
       <c r="F2" s="6">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="Q2" s="2" t="s">
         <v>0</v>
@@ -676,7 +676,7 @@
       </c>
       <c r="F3" t="str">
         <f>"S"&amp;F2</f>
-        <v>S23</v>
+        <v>S21</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>28</v>
@@ -751,7 +751,7 @@
       </c>
       <c r="F4" t="str">
         <f>F3&amp;"'"</f>
-        <v>S23'</v>
+        <v>S21'</v>
       </c>
       <c r="G4" t="str">
         <f>LEFT(G3,L3)&amp;TEXT(B4,"#0.0####")&amp;" "&amp;TEXT(C4,"#0.0####")&amp;" "&amp;TEXT(D4,"#0")&amp;")"</f>
@@ -948,7 +948,7 @@
       </c>
       <c r="F10" t="str">
         <f>"D"&amp;F2</f>
-        <v>D23</v>
+        <v>D21</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>24</v>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="F11" t="str">
         <f>F10&amp;"'"</f>
-        <v>D23'</v>
+        <v>D21'</v>
       </c>
       <c r="G11" t="str">
         <f>LEFT(G10,L10)&amp;TEXT(B11,"#0.0####")&amp;" "&amp;TEXT(C11,"#0.0####")&amp;" "&amp;TEXT(D11,"#0")&amp;")"</f>
@@ -1024,7 +1024,7 @@
       </c>
       <c r="F13" t="str">
         <f>"D"&amp;TEXT(F2+F16,"0")</f>
-        <v>D61</v>
+        <v>D59</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>25</v>
@@ -1077,7 +1077,7 @@
       </c>
       <c r="F14" t="str">
         <f>F13&amp;"'"</f>
-        <v>D61'</v>
+        <v>D59'</v>
       </c>
       <c r="G14" t="str">
         <f>LEFT(G13,L13)&amp;TEXT(B14,"#0.0####")&amp;" "&amp;TEXT(C14,"#0.0####")&amp;" "&amp;TEXT(D14,"#0")&amp;")"</f>
@@ -2269,7 +2269,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:V16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
renaming switches ahead of moving the nets
</commit_message>
<xml_diff>
--- a/KiCadHacks.xlsx
+++ b/KiCadHacks.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="11400" windowWidth="23720" windowHeight="5180"/>
+    <workbookView xWindow="0" yWindow="12000" windowWidth="23720" windowHeight="5180"/>
   </bookViews>
   <sheets>
     <sheet name="MoveSW" sheetId="1" r:id="rId1"/>
@@ -101,21 +101,6 @@
     <t xml:space="preserve">  (gr_line (start 65.562874 140.5122) (end 65.562873 165.108583) (layer Dwgs.User) (width 0.1))</t>
   </si>
   <si>
-    <t xml:space="preserve">    (at 144.907 96.9745 90)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    (at 149.987 100.086 270)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  (gr_line (start 156.386049 82.498785) (end 181.956049 82.498785) (layer Dwgs.User) (width 0.1))</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  (gr_line (start 181.956049 125.422785) (end 156.386049 125.422785) (layer Dwgs.User) (width 0.1))</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    (at 38.497 38.615 0)</t>
-  </si>
-  <si>
     <t xml:space="preserve">  (gr_line (start 65.562873 165.108583) (end 70.112873 169.658583) (layer Dwgs.User) (width 0.1))</t>
   </si>
   <si>
@@ -147,6 +132,21 @@
   </si>
   <si>
     <t xml:space="preserve">  (segment (start 159.536 121.261) (end 158.862 121.239) (width 0.1524) (layer Back) (net 91))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    (at 106.13048 123.75029 175)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  (gr_line (start 99.409328 120.251688) (end 98.903912 126.028621) (layer Dwgs.User) (width 0.1))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  (gr_line (start 112.851634 127.248888) (end 113.35705 121.471955) (layer Dwgs.User) (width 0.1))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    (at 103.03132 123.47915 175)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    (at 106.57323 118.68962 355)</t>
   </si>
 </sst>
 </file>
@@ -609,8 +609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -642,7 +642,7 @@
         <v>7</v>
       </c>
       <c r="F2" s="6">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="Q2" s="2" t="s">
         <v>0</v>
@@ -664,22 +664,22 @@
     <row r="3" spans="1:26" x14ac:dyDescent="0.35">
       <c r="B3">
         <f>IFERROR(VALUE(MID($G3,L3,M3-L3)),VALUE(RIGHT($G3,LEN($G3)-L3)))</f>
-        <v>38.497</v>
+        <v>106.13048000000001</v>
       </c>
       <c r="C3">
         <f t="shared" ref="C3" si="0">IFERROR(VALUE(MID($G3,M3,N3-M3)),VALUE(RIGHT($G3,LEN($G3)-M3)))</f>
-        <v>38.615000000000002</v>
+        <v>123.75029000000001</v>
       </c>
       <c r="D3">
         <f>IFERROR(VALUE(MID($G3,N3,O3-N3)),VALUE(MID($G3,N3,LEN($G3)-N3)))</f>
-        <v>0</v>
+        <v>175</v>
       </c>
       <c r="F3" t="str">
         <f>"S"&amp;F2</f>
-        <v>S21</v>
+        <v>S34</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="H3" s="1">
         <f>FIND(" ",$G3)</f>
@@ -703,11 +703,11 @@
       </c>
       <c r="M3" s="1">
         <f t="shared" ref="M3" si="4">FIND(" ",$G3,L3+1)</f>
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="N3" s="1">
         <f t="shared" ref="N3" si="5">FIND(" ",$G3,M3+1)</f>
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="O3" s="1" t="e">
         <f t="shared" ref="O3" si="6">FIND(" ",$G3,N3+1)</f>
@@ -715,18 +715,18 @@
       </c>
       <c r="Q3" s="9">
         <f>AVERAGE(Q6:Q9)</f>
-        <v>169.17104899999998</v>
+        <v>106.130481</v>
       </c>
       <c r="R3">
         <f>AVERAGE(R6:R9)</f>
-        <v>103.96078499999999</v>
+        <v>123.75028799999998</v>
       </c>
       <c r="S3">
         <f>ROUND(DEGREES(ASIN(R4/S4)),2)</f>
-        <v>-90</v>
+        <v>-5</v>
       </c>
       <c r="T3" s="1">
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="V3" s="1" t="s">
         <v>9</v>
@@ -739,35 +739,35 @@
     <row r="4" spans="1:26" x14ac:dyDescent="0.35">
       <c r="B4">
         <f>Q3</f>
-        <v>169.17104899999998</v>
+        <v>106.130481</v>
       </c>
       <c r="C4">
         <f>R3</f>
-        <v>103.96078499999999</v>
+        <v>123.75028799999998</v>
       </c>
       <c r="D4" s="7">
         <f>IF(S3+T3&lt;0,360+S3+T3,S3+T3)</f>
-        <v>270</v>
+        <v>175</v>
       </c>
       <c r="F4" t="str">
         <f>F3&amp;"'"</f>
-        <v>S21'</v>
+        <v>S34'</v>
       </c>
       <c r="G4" t="str">
         <f>LEFT(G3,L3)&amp;TEXT(B4,"#0.0####")&amp;" "&amp;TEXT(C4,"#0.0####")&amp;" "&amp;TEXT(D4,"#0")&amp;")"</f>
-        <v xml:space="preserve">    (at 169.17105 103.96079 270)</v>
+        <v xml:space="preserve">    (at 106.13048 123.75029 175)</v>
       </c>
       <c r="Q4" s="9">
         <f>IF(R6=R7,0,IF(R6&lt;R7,Q6,Q7))-IF(R8=R9,0,IF(R8&lt;R9,Q8,Q9))</f>
-        <v>0</v>
+        <v>-13.947721999999999</v>
       </c>
       <c r="R4" s="9">
         <f>IF(Q6=Q7,0,IF(Q6&lt;Q7,R6,R7))-IF(Q8=Q9,0,IF(Q8&lt;Q9,R8,R9))</f>
-        <v>-42.924000000000007</v>
+        <v>-1.2202669999999927</v>
       </c>
       <c r="S4" s="5">
         <f>SQRT(Q4^2+R4^2)</f>
-        <v>42.924000000000007</v>
+        <v>14.000999983593063</v>
       </c>
       <c r="V4" s="1"/>
       <c r="W4" s="1"/>
@@ -786,7 +786,7 @@
       </c>
       <c r="D5">
         <f>D4-D3</f>
-        <v>270</v>
+        <v>0</v>
       </c>
       <c r="H5" s="1" t="e">
         <f>FIND(" ",$G5)</f>
@@ -804,26 +804,26 @@
     <row r="6" spans="1:26" x14ac:dyDescent="0.35">
       <c r="B6" s="5">
         <f>B4-B3</f>
-        <v>130.67404899999997</v>
+        <v>9.9999999747524271E-7</v>
       </c>
       <c r="C6" s="5">
         <f>C4-C3</f>
-        <v>65.345784999999978</v>
+        <v>-2.0000000233721948E-6</v>
       </c>
       <c r="D6" s="5">
         <f>ROUND(S3,2)</f>
-        <v>-90</v>
+        <v>-5</v>
       </c>
       <c r="Q6" s="9">
         <f>VALUE(MID($U$6,V6+1,W6-V6))</f>
-        <v>156.38604900000001</v>
+        <v>99.409328000000002</v>
       </c>
       <c r="R6" s="9">
         <f>VALUE(MID($U$6,W6+1,X6-W6-1))</f>
-        <v>82.498784999999998</v>
+        <v>120.251688</v>
       </c>
       <c r="U6" s="1" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="V6" s="1">
         <f>FIND(V2,$U$6)+LEN(V2)</f>
@@ -831,7 +831,7 @@
       </c>
       <c r="W6" s="1">
         <f>FIND(" ",$U$6,V6+1)</f>
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="X6" s="1">
         <f>FIND(")",$U$6,W6+1)</f>
@@ -841,23 +841,23 @@
     <row r="7" spans="1:26" x14ac:dyDescent="0.35">
       <c r="B7" s="5">
         <f>B10-B3</f>
-        <v>106.41000000000001</v>
+        <v>-3.0991600000000119</v>
       </c>
       <c r="C7" s="5">
         <f>C10-C3</f>
-        <v>58.359500000000004</v>
+        <v>-0.2711400000000026</v>
       </c>
       <c r="D7" s="5">
         <f>SQRT(B7^2+C7^2)</f>
-        <v>121.36275928080245</v>
+        <v>3.1109981686269239</v>
       </c>
       <c r="Q7" s="9">
         <f>VALUE(MID($U$6,V7+1,W7-V7))</f>
-        <v>181.95604900000001</v>
+        <v>98.903912000000005</v>
       </c>
       <c r="R7" s="9">
         <f>VALUE(MID($U$6,W7+1,X7-W7-1))</f>
-        <v>82.498784999999998</v>
+        <v>126.028621</v>
       </c>
       <c r="V7" s="1">
         <f>FIND(V3,$U$6)+LEN(V3)</f>
@@ -865,7 +865,7 @@
       </c>
       <c r="W7" s="1">
         <f>FIND(" ",$U$6,V7+1)</f>
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="X7" s="1">
         <f>FIND(")",$U$6,W7+1)</f>
@@ -875,11 +875,11 @@
     <row r="8" spans="1:26" x14ac:dyDescent="0.35">
       <c r="B8" s="5">
         <f>$D7*COS(RADIANS($D4))</f>
-        <v>-2.2303109552448287E-14</v>
+        <v>-3.0991598813592716</v>
       </c>
       <c r="C8" s="5">
         <f>-$D7*SIN(RADIANS($D4))</f>
-        <v>121.36275928080245</v>
+        <v>-0.27114135607328393</v>
       </c>
       <c r="E8" s="1">
         <f>IF(AND(D5&lt;0,B7&lt;1,B7&lt;C7),-1,1)</f>
@@ -887,14 +887,14 @@
       </c>
       <c r="Q8" s="9">
         <f>VALUE(MID($U$8,V8+1,W8-V8))</f>
-        <v>181.95604900000001</v>
+        <v>112.851634</v>
       </c>
       <c r="R8" s="9">
         <f>VALUE(MID($U$8,W8+1,X8-W8-1))</f>
-        <v>125.422785</v>
+        <v>127.24888799999999</v>
       </c>
       <c r="U8" s="1" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="V8" s="1">
         <f>FIND(V2,$U$8)+LEN(V2)</f>
@@ -914,11 +914,11 @@
       <c r="C9" s="5"/>
       <c r="Q9" s="9">
         <f>VALUE(MID($U$8,V9+1,W9-V9))</f>
-        <v>156.38604900000001</v>
+        <v>113.35705</v>
       </c>
       <c r="R9" s="9">
         <f>VALUE(MID($U$8,W9+1,X9-W9-1))</f>
-        <v>125.422785</v>
+        <v>121.47195499999999</v>
       </c>
       <c r="V9" s="1">
         <f>FIND(V3,$U$8)+LEN(V3)</f>
@@ -926,32 +926,32 @@
       </c>
       <c r="W9" s="1">
         <f>FIND(" ",$U$8,V9+1)</f>
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="X9" s="1">
         <f>FIND(")",$U$8,W9+1)</f>
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.35">
       <c r="B10">
         <f>IFERROR(VALUE(MID($G10,L10,M10-L10)),VALUE(RIGHT($G10,LEN($G10)-L10)))</f>
-        <v>144.90700000000001</v>
+        <v>103.03131999999999</v>
       </c>
       <c r="C10">
         <f t="shared" ref="C10" si="7">IFERROR(VALUE(MID($G10,M10,N10-M10)),VALUE(RIGHT($G10,LEN($G10)-M10)))</f>
-        <v>96.974500000000006</v>
+        <v>123.47915</v>
       </c>
       <c r="D10">
         <f>IFERROR(VALUE(MID($G10,N10,O10-N10)),VALUE(MID($G10,N10,LEN($G10)-N10)))</f>
-        <v>90</v>
+        <v>175</v>
       </c>
       <c r="F10" t="str">
         <f>"D"&amp;F2</f>
-        <v>D21</v>
+        <v>D34</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="H10" s="1">
         <f>FIND(" ",$G10)</f>
@@ -975,11 +975,11 @@
       </c>
       <c r="M10" s="1">
         <f t="shared" si="8"/>
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="N10" s="1">
         <f t="shared" si="8"/>
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="O10" s="1" t="e">
         <f t="shared" si="8"/>
@@ -989,45 +989,53 @@
     <row r="11" spans="1:26" x14ac:dyDescent="0.35">
       <c r="B11">
         <f>B4+B8</f>
-        <v>169.17104899999995</v>
+        <v>103.03132111864073</v>
       </c>
       <c r="C11">
         <f>C4+C8</f>
-        <v>225.32354428080242</v>
+        <v>123.4791466439267</v>
       </c>
       <c r="D11">
         <f>IF(D10+D$5&lt;0,360+D10+D$5,D10+D$5)</f>
-        <v>360</v>
+        <v>175</v>
       </c>
       <c r="F11" t="str">
         <f>F10&amp;"'"</f>
-        <v>D21'</v>
+        <v>D34'</v>
       </c>
       <c r="G11" t="str">
         <f>LEFT(G10,L10)&amp;TEXT(B11,"#0.0####")&amp;" "&amp;TEXT(C11,"#0.0####")&amp;" "&amp;TEXT(D11,"#0")&amp;")"</f>
-        <v xml:space="preserve">    (at 169.17105 225.32354 360)</v>
+        <v xml:space="preserve">    (at 103.03132 123.47915 175)</v>
       </c>
       <c r="V11" s="8"/>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="Q12">
+        <v>30</v>
+      </c>
+      <c r="R12">
+        <v>68</v>
+      </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.35">
       <c r="B13">
         <f>IFERROR(VALUE(MID($G13,L13,M13-L13)),VALUE(RIGHT($G13,LEN($G13)-L13)))</f>
-        <v>149.98699999999999</v>
+        <v>106.57323</v>
       </c>
       <c r="C13">
         <f t="shared" ref="C13" si="9">IFERROR(VALUE(MID($G13,M13,N13-M13)),VALUE(RIGHT($G13,LEN($G13)-M13)))</f>
-        <v>100.086</v>
+        <v>118.68962000000001</v>
       </c>
       <c r="D13">
         <f>IFERROR(VALUE(MID($G13,N13,O13-N13)),VALUE(MID($G13,N13,LEN($G13)-N13)))</f>
-        <v>270</v>
+        <v>355</v>
       </c>
       <c r="F13" t="str">
         <f>"D"&amp;TEXT(F2+F16,"0")</f>
-        <v>D59</v>
+        <v>D72</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="H13" s="1">
         <f>FIND(" ",$G13)</f>
@@ -1051,11 +1059,11 @@
       </c>
       <c r="M13" s="1">
         <f t="shared" si="10"/>
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="N13" s="1">
         <f t="shared" si="10"/>
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="O13" s="1" t="e">
         <f t="shared" si="10"/>
@@ -1065,29 +1073,29 @@
     <row r="14" spans="1:26" x14ac:dyDescent="0.35">
       <c r="B14">
         <f>B4+B17</f>
-        <v>169.17104899999998</v>
+        <v>106.5732321731581</v>
       </c>
       <c r="C14">
         <f>C4+C17</f>
-        <v>109.04078499999999</v>
+        <v>118.68961893369392</v>
       </c>
       <c r="D14">
         <f>IF(D13+D$5&lt;0,360+D13+D$5,D13+D$5)</f>
-        <v>540</v>
+        <v>355</v>
       </c>
       <c r="F14" t="str">
         <f>F13&amp;"'"</f>
-        <v>D59'</v>
+        <v>D72'</v>
       </c>
       <c r="G14" t="str">
         <f>LEFT(G13,L13)&amp;TEXT(B14,"#0.0####")&amp;" "&amp;TEXT(C14,"#0.0####")&amp;" "&amp;TEXT(D14,"#0")&amp;")"</f>
-        <v xml:space="preserve">    (at 169.17105 109.04079 540)</v>
+        <v xml:space="preserve">    (at 106.57323 118.68962 355)</v>
       </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.35">
       <c r="D15">
         <f>90+D6</f>
-        <v>0</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.35">
@@ -1111,11 +1119,11 @@
       <c r="A17" s="1"/>
       <c r="B17" s="5">
         <f>-$D16*SIN(RADIANS($D14))</f>
-        <v>-1.8671262452807362E-15</v>
+        <v>0.44275117315810408</v>
       </c>
       <c r="C17" s="5">
         <f>-E17*$D16*COS(RADIANS($D14))</f>
-        <v>5.0799999999999983</v>
+        <v>-5.0606690663060654</v>
       </c>
       <c r="E17" s="1">
         <f>IF(AND(D5&lt;0,B7&lt;1,B7&lt;C7),-1,1)</f>
@@ -1612,7 +1620,7 @@
       </c>
       <c r="Y10">
         <f>MIN(MoveSW!Q6:Q9)</f>
-        <v>156.38604900000001</v>
+        <v>98.903912000000005</v>
       </c>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.35">
@@ -1633,7 +1641,7 @@
       </c>
       <c r="Y11">
         <f>MAX(MoveSW!Q6:Q9)</f>
-        <v>181.95604900000001</v>
+        <v>113.35705</v>
       </c>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.35">
@@ -1654,7 +1662,7 @@
         <v>169.65858299999999</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="H12" s="1">
         <f t="shared" si="1"/>
@@ -1722,7 +1730,7 @@
       </c>
       <c r="Y12">
         <f>Y11-Y10</f>
-        <v>25.569999999999993</v>
+        <v>14.453137999999996</v>
       </c>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.35">
@@ -1743,7 +1751,7 @@
         <v>170.815</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="H13" s="1">
         <f t="shared" si="1"/>
@@ -2370,10 +2378,10 @@
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="H3" s="12">
         <f>FIND(H$1,$G3)</f>
@@ -2401,7 +2409,7 @@
       </c>
       <c r="O3" s="12"/>
       <c r="P3" s="10" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="2:22" x14ac:dyDescent="0.35">
@@ -2418,10 +2426,10 @@
         <v>270</v>
       </c>
       <c r="E4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="H4" s="12">
         <f>FIND(H$1,$G4)</f>
@@ -2487,10 +2495,10 @@
         <v>180</v>
       </c>
       <c r="E5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="G5" s="17" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="H5" s="12">
         <f>FIND(H$1,$G5)</f>
@@ -2645,7 +2653,7 @@
       </c>
       <c r="O12" s="12"/>
       <c r="P12" s="10" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="2:22" x14ac:dyDescent="0.35">
@@ -2704,7 +2712,7 @@
       </c>
       <c r="O15" s="12"/>
       <c r="P15" s="10" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="2:22" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
realigned the nets to match the reordered switches
</commit_message>
<xml_diff>
--- a/KiCadHacks.xlsx
+++ b/KiCadHacks.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="12000" windowWidth="23720" windowHeight="5180"/>
+    <workbookView xWindow="0" yWindow="12600" windowWidth="23720" windowHeight="5180"/>
   </bookViews>
   <sheets>
     <sheet name="MoveSW" sheetId="1" r:id="rId1"/>
@@ -125,28 +125,28 @@
     <t xml:space="preserve">    (at 55.753 41.021 180)</t>
   </si>
   <si>
-    <t xml:space="preserve">  (segment (start 158.786 121.239) (end 155.98 121.239) (width 0.1524) (layer Back) (net 91))</t>
-  </si>
-  <si>
     <t xml:space="preserve">  (segment (start 55.797 36.665) (end 55.775 37.3388) (width 0.1524) (layer Back) (net 91))</t>
   </si>
   <si>
-    <t xml:space="preserve">  (segment (start 159.536 121.261) (end 158.862 121.239) (width 0.1524) (layer Back) (net 91))</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    (at 106.13048 123.75029 175)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  (gr_line (start 99.409328 120.251688) (end 98.903912 126.028621) (layer Dwgs.User) (width 0.1))</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  (gr_line (start 112.851634 127.248888) (end 113.35705 121.471955) (layer Dwgs.User) (width 0.1))</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    (at 103.03132 123.47915 175)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    (at 106.57323 118.68962 355)</t>
+    <t xml:space="preserve">    (at 145.20637 157.41722 370)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    (at 143.02472 162.96027 190)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    (at 146.08851 162.42005 190)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  (gr_line (start 138.690866 160.780219) (end 139.697852 166.491119) (layer Dwgs.User) (width 0.1))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  (gr_line (start 153.486145 164.059871) (end 152.47916 158.348971) (layer Dwgs.User) (width 0.1))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  (gr_line (start 176 163.422) (end 176 133.026) (angle 90) (layer Edge.Cuts) (width 0.127))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  (gr_line (start 177.828 133.026) (end 173.279 128.477) (angle 90) (layer Edge.Cuts) (width 0.127))</t>
   </si>
 </sst>
 </file>
@@ -609,8 +609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="Q36" sqref="Q12:S36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -642,7 +642,7 @@
         <v>7</v>
       </c>
       <c r="F2" s="6">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="Q2" s="2" t="s">
         <v>0</v>
@@ -664,19 +664,19 @@
     <row r="3" spans="1:26" x14ac:dyDescent="0.35">
       <c r="B3">
         <f>IFERROR(VALUE(MID($G3,L3,M3-L3)),VALUE(RIGHT($G3,LEN($G3)-L3)))</f>
-        <v>106.13048000000001</v>
+        <v>146.08851000000001</v>
       </c>
       <c r="C3">
         <f t="shared" ref="C3" si="0">IFERROR(VALUE(MID($G3,M3,N3-M3)),VALUE(RIGHT($G3,LEN($G3)-M3)))</f>
-        <v>123.75029000000001</v>
+        <v>162.42005</v>
       </c>
       <c r="D3">
         <f>IFERROR(VALUE(MID($G3,N3,O3-N3)),VALUE(MID($G3,N3,LEN($G3)-N3)))</f>
-        <v>175</v>
+        <v>190</v>
       </c>
       <c r="F3" t="str">
         <f>"S"&amp;F2</f>
-        <v>S34</v>
+        <v>S29</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>35</v>
@@ -715,15 +715,15 @@
       </c>
       <c r="Q3" s="9">
         <f>AVERAGE(Q6:Q9)</f>
-        <v>106.130481</v>
+        <v>146.08850575</v>
       </c>
       <c r="R3">
         <f>AVERAGE(R6:R9)</f>
-        <v>123.75028799999998</v>
+        <v>162.42004500000002</v>
       </c>
       <c r="S3">
         <f>ROUND(DEGREES(ASIN(R4/S4)),2)</f>
-        <v>-5</v>
+        <v>10</v>
       </c>
       <c r="T3" s="1">
         <v>180</v>
@@ -739,35 +739,35 @@
     <row r="4" spans="1:26" x14ac:dyDescent="0.35">
       <c r="B4">
         <f>Q3</f>
-        <v>106.130481</v>
+        <v>146.08850575</v>
       </c>
       <c r="C4">
         <f>R3</f>
-        <v>123.75028799999998</v>
+        <v>162.42004500000002</v>
       </c>
       <c r="D4" s="7">
         <f>IF(S3+T3&lt;0,360+S3+T3,S3+T3)</f>
-        <v>175</v>
+        <v>190</v>
       </c>
       <c r="F4" t="str">
         <f>F3&amp;"'"</f>
-        <v>S34'</v>
+        <v>S29'</v>
       </c>
       <c r="G4" t="str">
         <f>LEFT(G3,L3)&amp;TEXT(B4,"#0.0####")&amp;" "&amp;TEXT(C4,"#0.0####")&amp;" "&amp;TEXT(D4,"#0")&amp;")"</f>
-        <v xml:space="preserve">    (at 106.13048 123.75029 175)</v>
+        <v xml:space="preserve">    (at 146.08851 162.42005 190)</v>
       </c>
       <c r="Q4" s="9">
         <f>IF(R6=R7,0,IF(R6&lt;R7,Q6,Q7))-IF(R8=R9,0,IF(R8&lt;R9,Q8,Q9))</f>
-        <v>-13.947721999999999</v>
+        <v>-13.788294000000008</v>
       </c>
       <c r="R4" s="9">
         <f>IF(Q6=Q7,0,IF(Q6&lt;Q7,R6,R7))-IF(Q8=Q9,0,IF(Q8&lt;Q9,R8,R9))</f>
-        <v>-1.2202669999999927</v>
+        <v>2.4312479999999823</v>
       </c>
       <c r="S4" s="5">
         <f>SQRT(Q4^2+R4^2)</f>
-        <v>14.000999983593063</v>
+        <v>14.001000616668087</v>
       </c>
       <c r="V4" s="1"/>
       <c r="W4" s="1"/>
@@ -804,23 +804,23 @@
     <row r="6" spans="1:26" x14ac:dyDescent="0.35">
       <c r="B6" s="5">
         <f>B4-B3</f>
-        <v>9.9999999747524271E-7</v>
+        <v>-4.2500000176914909E-6</v>
       </c>
       <c r="C6" s="5">
         <f>C4-C3</f>
-        <v>-2.0000000233721948E-6</v>
+        <v>-4.9999999873762135E-6</v>
       </c>
       <c r="D6" s="5">
         <f>ROUND(S3,2)</f>
-        <v>-5</v>
+        <v>10</v>
       </c>
       <c r="Q6" s="9">
         <f>VALUE(MID($U$6,V6+1,W6-V6))</f>
-        <v>99.409328000000002</v>
+        <v>138.690866</v>
       </c>
       <c r="R6" s="9">
         <f>VALUE(MID($U$6,W6+1,X6-W6-1))</f>
-        <v>120.251688</v>
+        <v>160.78021899999999</v>
       </c>
       <c r="U6" s="1" t="s">
         <v>36</v>
@@ -831,55 +831,55 @@
       </c>
       <c r="W6" s="1">
         <f>FIND(" ",$U$6,V6+1)</f>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="X6" s="1">
         <f>FIND(")",$U$6,W6+1)</f>
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.35">
       <c r="B7" s="5">
         <f>B10-B3</f>
-        <v>-3.0991600000000119</v>
+        <v>-3.0637900000000116</v>
       </c>
       <c r="C7" s="5">
         <f>C10-C3</f>
-        <v>-0.2711400000000026</v>
+        <v>0.54022000000000503</v>
       </c>
       <c r="D7" s="5">
         <f>SQRT(B7^2+C7^2)</f>
-        <v>3.1109981686269239</v>
+        <v>3.1110523641526955</v>
       </c>
       <c r="Q7" s="9">
         <f>VALUE(MID($U$6,V7+1,W7-V7))</f>
-        <v>98.903912000000005</v>
+        <v>139.69785200000001</v>
       </c>
       <c r="R7" s="9">
         <f>VALUE(MID($U$6,W7+1,X7-W7-1))</f>
-        <v>126.028621</v>
+        <v>166.491119</v>
       </c>
       <c r="V7" s="1">
         <f>FIND(V3,$U$6)+LEN(V3)</f>
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="W7" s="1">
         <f>FIND(" ",$U$6,V7+1)</f>
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="X7" s="1">
         <f>FIND(")",$U$6,W7+1)</f>
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.35">
       <c r="B8" s="5">
         <f>$D7*COS(RADIANS($D4))</f>
-        <v>-3.0991598813592716</v>
+        <v>-3.0637884882445334</v>
       </c>
       <c r="C8" s="5">
         <f>-$D7*SIN(RADIANS($D4))</f>
-        <v>-0.27114135607328393</v>
+        <v>0.54022857366151134</v>
       </c>
       <c r="E8" s="1">
         <f>IF(AND(D5&lt;0,B7&lt;1,B7&lt;C7),-1,1)</f>
@@ -887,11 +887,11 @@
       </c>
       <c r="Q8" s="9">
         <f>VALUE(MID($U$8,V8+1,W8-V8))</f>
-        <v>112.851634</v>
+        <v>153.48614499999999</v>
       </c>
       <c r="R8" s="9">
         <f>VALUE(MID($U$8,W8+1,X8-W8-1))</f>
-        <v>127.24888799999999</v>
+        <v>164.05987099999999</v>
       </c>
       <c r="U8" s="1" t="s">
         <v>37</v>
@@ -914,11 +914,11 @@
       <c r="C9" s="5"/>
       <c r="Q9" s="9">
         <f>VALUE(MID($U$8,V9+1,W9-V9))</f>
-        <v>113.35705</v>
+        <v>152.47916000000001</v>
       </c>
       <c r="R9" s="9">
         <f>VALUE(MID($U$8,W9+1,X9-W9-1))</f>
-        <v>121.47195499999999</v>
+        <v>158.34897100000001</v>
       </c>
       <c r="V9" s="1">
         <f>FIND(V3,$U$8)+LEN(V3)</f>
@@ -936,22 +936,22 @@
     <row r="10" spans="1:26" x14ac:dyDescent="0.35">
       <c r="B10">
         <f>IFERROR(VALUE(MID($G10,L10,M10-L10)),VALUE(RIGHT($G10,LEN($G10)-L10)))</f>
-        <v>103.03131999999999</v>
+        <v>143.02472</v>
       </c>
       <c r="C10">
         <f t="shared" ref="C10" si="7">IFERROR(VALUE(MID($G10,M10,N10-M10)),VALUE(RIGHT($G10,LEN($G10)-M10)))</f>
-        <v>123.47915</v>
+        <v>162.96027000000001</v>
       </c>
       <c r="D10">
         <f>IFERROR(VALUE(MID($G10,N10,O10-N10)),VALUE(MID($G10,N10,LEN($G10)-N10)))</f>
-        <v>175</v>
+        <v>190</v>
       </c>
       <c r="F10" t="str">
         <f>"D"&amp;F2</f>
-        <v>D34</v>
+        <v>D29</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="H10" s="1">
         <f>FIND(" ",$G10)</f>
@@ -989,53 +989,45 @@
     <row r="11" spans="1:26" x14ac:dyDescent="0.35">
       <c r="B11">
         <f>B4+B8</f>
-        <v>103.03132111864073</v>
+        <v>143.02471726175546</v>
       </c>
       <c r="C11">
         <f>C4+C8</f>
-        <v>123.4791466439267</v>
+        <v>162.96027357366154</v>
       </c>
       <c r="D11">
         <f>IF(D10+D$5&lt;0,360+D10+D$5,D10+D$5)</f>
-        <v>175</v>
+        <v>190</v>
       </c>
       <c r="F11" t="str">
         <f>F10&amp;"'"</f>
-        <v>D34'</v>
+        <v>D29'</v>
       </c>
       <c r="G11" t="str">
         <f>LEFT(G10,L10)&amp;TEXT(B11,"#0.0####")&amp;" "&amp;TEXT(C11,"#0.0####")&amp;" "&amp;TEXT(D11,"#0")&amp;")"</f>
-        <v xml:space="preserve">    (at 103.03132 123.47915 175)</v>
+        <v xml:space="preserve">    (at 143.02472 162.96027 190)</v>
       </c>
       <c r="V11" s="8"/>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="Q12">
-        <v>30</v>
-      </c>
-      <c r="R12">
-        <v>68</v>
-      </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.35">
       <c r="B13">
         <f>IFERROR(VALUE(MID($G13,L13,M13-L13)),VALUE(RIGHT($G13,LEN($G13)-L13)))</f>
-        <v>106.57323</v>
+        <v>145.20636999999999</v>
       </c>
       <c r="C13">
         <f t="shared" ref="C13" si="9">IFERROR(VALUE(MID($G13,M13,N13-M13)),VALUE(RIGHT($G13,LEN($G13)-M13)))</f>
-        <v>118.68962000000001</v>
+        <v>157.41721999999999</v>
       </c>
       <c r="D13">
         <f>IFERROR(VALUE(MID($G13,N13,O13-N13)),VALUE(MID($G13,N13,LEN($G13)-N13)))</f>
-        <v>355</v>
+        <v>370</v>
       </c>
       <c r="F13" t="str">
         <f>"D"&amp;TEXT(F2+F16,"0")</f>
-        <v>D72</v>
+        <v>D67</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="H13" s="1">
         <f>FIND(" ",$G13)</f>
@@ -1073,29 +1065,29 @@
     <row r="14" spans="1:26" x14ac:dyDescent="0.35">
       <c r="B14">
         <f>B4+B17</f>
-        <v>106.5732321731581</v>
+        <v>145.20637300745199</v>
       </c>
       <c r="C14">
         <f>C4+C17</f>
-        <v>118.68961893369392</v>
+        <v>157.41722161469801</v>
       </c>
       <c r="D14">
         <f>IF(D13+D$5&lt;0,360+D13+D$5,D13+D$5)</f>
-        <v>355</v>
+        <v>370</v>
       </c>
       <c r="F14" t="str">
         <f>F13&amp;"'"</f>
-        <v>D72'</v>
+        <v>D67'</v>
       </c>
       <c r="G14" t="str">
         <f>LEFT(G13,L13)&amp;TEXT(B14,"#0.0####")&amp;" "&amp;TEXT(C14,"#0.0####")&amp;" "&amp;TEXT(D14,"#0")&amp;")"</f>
-        <v xml:space="preserve">    (at 106.57323 118.68962 355)</v>
+        <v xml:space="preserve">    (at 145.20637 157.41722 370)</v>
       </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.35">
       <c r="D15">
         <f>90+D6</f>
-        <v>85</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.35">
@@ -1119,11 +1111,11 @@
       <c r="A17" s="1"/>
       <c r="B17" s="5">
         <f>-$D16*SIN(RADIANS($D14))</f>
-        <v>0.44275117315810408</v>
+        <v>-0.88213274254800367</v>
       </c>
       <c r="C17" s="5">
         <f>-E17*$D16*COS(RADIANS($D14))</f>
-        <v>-5.0606690663060654</v>
+        <v>-5.0028233853020154</v>
       </c>
       <c r="E17" s="1">
         <f>IF(AND(D5&lt;0,B7&lt;1,B7&lt;C7),-1,1)</f>
@@ -1620,7 +1612,7 @@
       </c>
       <c r="Y10">
         <f>MIN(MoveSW!Q6:Q9)</f>
-        <v>98.903912000000005</v>
+        <v>138.690866</v>
       </c>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.35">
@@ -1641,7 +1633,7 @@
       </c>
       <c r="Y11">
         <f>MAX(MoveSW!Q6:Q9)</f>
-        <v>113.35705</v>
+        <v>153.48614499999999</v>
       </c>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.35">
@@ -1730,7 +1722,7 @@
       </c>
       <c r="Y12">
         <f>Y11-Y10</f>
-        <v>14.453137999999996</v>
+        <v>14.795278999999994</v>
       </c>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.35">
@@ -2278,7 +2270,7 @@
   <dimension ref="B1:V16"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2409,7 +2401,7 @@
       </c>
       <c r="O3" s="12"/>
       <c r="P3" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="2:22" x14ac:dyDescent="0.35">
@@ -2645,25 +2637,25 @@
     <row r="12" spans="2:22" x14ac:dyDescent="0.35">
       <c r="M12">
         <f>VALUE(MID($P12,Q13+LEN(Q$1),R13-Q13-LEN(Q$1)))</f>
-        <v>159.536</v>
+        <v>176</v>
       </c>
       <c r="N12">
         <f>VALUE(MID($P12,R13+LEN(R$1),S13-R13-LEN(R$1)))</f>
-        <v>121.261</v>
+        <v>163.422</v>
       </c>
       <c r="O12" s="12"/>
       <c r="P12" s="10" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="2:22" x14ac:dyDescent="0.35">
       <c r="M13">
         <f>VALUE(MID($P12,T13+LEN(T$1),U13-T13-LEN(T$1)))</f>
-        <v>158.86199999999999</v>
+        <v>176</v>
       </c>
       <c r="N13">
         <f>VALUE(MID($P12,U13+LEN(U$1),V13-U13-LEN(U$1)))</f>
-        <v>121.239</v>
+        <v>133.02600000000001</v>
       </c>
       <c r="O13" s="12"/>
       <c r="Q13" s="12">
@@ -2672,57 +2664,57 @@
       </c>
       <c r="R13" s="12">
         <f>FIND(R$1,$P12,Q13+LEN(Q$1))</f>
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="S13" s="12">
         <f>FIND(S$1,$P12,R13+LEN(R$1))</f>
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="T13" s="12">
         <f>FIND(T$1,$P12)</f>
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="U13" s="12">
         <f>FIND(U$1,$P12,T13+LEN(T$1))</f>
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="V13" s="12">
         <f>FIND(V$1,$P12,U13+LEN(U$1))</f>
-        <v>56</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="2:22" x14ac:dyDescent="0.35">
       <c r="M14" s="12">
         <f>ROUND(((M12*N13-M13*N12)*(M15-M16)-(M12-M13)*(M15*N16-N15*M16))/((M12-M13)*(N15-N16)-(N12-N13)*(M15-M16)),3)</f>
-        <v>158.86199999999999</v>
+        <v>176</v>
       </c>
       <c r="N14" s="12">
         <f>ROUND(((M12*N13-M13*N12)*(N15-N16)-(N12-N13)*(M15*N16-N15*M16))/((M12-M13)*(N15-N16)-(N12-N13)*(M15-M16)),3)</f>
-        <v>121.239</v>
+        <v>131.19800000000001</v>
       </c>
     </row>
     <row r="15" spans="2:22" x14ac:dyDescent="0.35">
       <c r="M15">
         <f>VALUE(MID($P15,Q16+LEN(Q$1),R16-Q16-LEN(Q$1)))</f>
-        <v>158.786</v>
+        <v>177.828</v>
       </c>
       <c r="N15">
         <f>VALUE(MID($P15,R16+LEN(R$1),S16-R16-LEN(R$1)))</f>
-        <v>121.239</v>
+        <v>133.02600000000001</v>
       </c>
       <c r="O15" s="12"/>
       <c r="P15" s="10" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="2:22" x14ac:dyDescent="0.35">
       <c r="M16">
         <f>VALUE(MID($P15,T16+LEN(T$1),U16-T16-LEN(T$1)))</f>
-        <v>155.97999999999999</v>
+        <v>173.279</v>
       </c>
       <c r="N16">
         <f>VALUE(MID($P15,U16+LEN(U$1),V16-U16-LEN(U$1)))</f>
-        <v>121.239</v>
+        <v>128.477</v>
       </c>
       <c r="O16" s="12"/>
       <c r="Q16" s="12">
@@ -2743,11 +2735,11 @@
       </c>
       <c r="U16" s="12">
         <f>FIND(U$1,$P15,T16+LEN(T$1))</f>
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="V16" s="12">
         <f>FIND(V$1,$P15,U16+LEN(U$1))</f>
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
reorderd the row and column nets
</commit_message>
<xml_diff>
--- a/KiCadHacks.xlsx
+++ b/KiCadHacks.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="12600" windowWidth="23720" windowHeight="5180"/>
+    <workbookView xWindow="0" yWindow="13200" windowWidth="23720" windowHeight="5180"/>
   </bookViews>
   <sheets>
     <sheet name="MoveSW" sheetId="1" r:id="rId1"/>
@@ -609,21 +609,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="Q36" sqref="Q12:S36"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S1" sqref="S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="2.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="2.26953125" customWidth="1"/>
+    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="1.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.90625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="2.54296875" style="1" customWidth="1"/>
     <col min="11" max="15" width="2.54296875" customWidth="1"/>
     <col min="16" max="16" width="2" customWidth="1"/>
-    <col min="17" max="18" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="3.26953125" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="3.54296875" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="67.6328125" bestFit="1" customWidth="1"/>
     <col min="22" max="24" width="2.54296875" customWidth="1"/>
     <col min="25" max="25" width="2.453125" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
Completed movement of switches into row-column grid.
</commit_message>
<xml_diff>
--- a/KiCadHacks.xlsx
+++ b/KiCadHacks.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="13200" windowWidth="23720" windowHeight="5180"/>
+    <workbookView xWindow="0" yWindow="13800" windowWidth="23720" windowHeight="5180"/>
   </bookViews>
   <sheets>
     <sheet name="MoveSW" sheetId="1" r:id="rId1"/>
@@ -609,8 +609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S1" sqref="S1"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1014,6 +1014,14 @@
       </c>
       <c r="V11" s="8"/>
     </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="Q12">
+        <v>4700</v>
+      </c>
+      <c r="R12">
+        <v>4650</v>
+      </c>
+    </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.35">
       <c r="B13">
         <f>IFERROR(VALUE(MID($G13,L13,M13-L13)),VALUE(RIGHT($G13,LEN($G13)-L13)))</f>
@@ -1066,6 +1074,14 @@
         <f t="shared" si="10"/>
         <v>#VALUE!</v>
       </c>
+      <c r="Q13">
+        <f>Q12+200</f>
+        <v>4900</v>
+      </c>
+      <c r="R13">
+        <f>R12+200</f>
+        <v>4850</v>
+      </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.35">
       <c r="B14">
@@ -1094,6 +1110,13 @@
         <f>90+D6</f>
         <v>100</v>
       </c>
+      <c r="Q15">
+        <v>6800</v>
+      </c>
+      <c r="R15">
+        <f>R12+700</f>
+        <v>5350</v>
+      </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A16" s="5"/>
@@ -1110,6 +1133,14 @@
       <c r="F16" s="1">
         <f>74-36</f>
         <v>38</v>
+      </c>
+      <c r="Q16">
+        <f>Q15+200</f>
+        <v>7000</v>
+      </c>
+      <c r="R16">
+        <f>R15+200</f>
+        <v>5550</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>